<commit_message>
Atualizado por script em 08-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/brazil_serie-b_2023.xlsx
+++ b/2023/brazil_serie-b_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V349"/>
+  <dimension ref="A1:V351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2597,19 +2597,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
         <v>2.2</v>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>2.43</v>
+        <v>2.37</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:57</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.09</v>
+        <v>3.04</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:51</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.54</v>
+        <v>3.84</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>3.46</v>
+        <v>3.52</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:57</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-crb/jah69YO2/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ponte-preta/vZ3M5jOR/</t>
         </is>
       </c>
     </row>
@@ -2689,19 +2689,19 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>2.2</v>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>2.37</v>
+        <v>2.43</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:57</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>3.04</v>
+        <v>3.09</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:51</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>3.84</v>
+        <v>3.54</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>3.52</v>
+        <v>3.46</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:57</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ponte-preta/vZ3M5jOR/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-crb/jah69YO2/</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1.92</v>
+        <v>2.15</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.86</v>
+        <v>2.03</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:59</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.33</v>
+        <v>3.06</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,15 +3280,15 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.51</v>
+        <v>3.25</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:57</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>4.47</v>
+        <v>3.72</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,16 +3296,16 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>4.68</v>
+        <v>4.28</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:59</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-sampaio-correa/pf7UaLi6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-botafogo-sp/xAqcal1e/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>2.15</v>
+        <v>1.92</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.03</v>
+        <v>1.86</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:59</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.06</v>
+        <v>3.33</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>3.25</v>
+        <v>3.51</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:57</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.72</v>
+        <v>4.47</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>4.28</v>
+        <v>4.68</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:59</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-botafogo-sp/xAqcal1e/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-sampaio-correa/pf7UaLi6/</t>
         </is>
       </c>
     </row>
@@ -4069,71 +4069,71 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="I40" t="n">
         <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>2.2</v>
+        <v>2.07</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>06/05/2023 15:09</t>
         </is>
       </c>
       <c r="L40" t="n">
-        <v>2.03</v>
+        <v>1.95</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>06/05/2023 23:13</t>
+          <t>06/05/2023 23:09</t>
         </is>
       </c>
       <c r="N40" t="n">
-        <v>3.21</v>
+        <v>3.06</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>06/05/2023 15:09</t>
         </is>
       </c>
       <c r="P40" t="n">
-        <v>3.32</v>
+        <v>3.3</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>06/05/2023 23:13</t>
+          <t>06/05/2023 23:10</t>
         </is>
       </c>
       <c r="R40" t="n">
-        <v>3.4</v>
+        <v>3.96</v>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>06/05/2023 15:09</t>
         </is>
       </c>
       <c r="T40" t="n">
-        <v>4.16</v>
+        <v>4.55</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>06/05/2023 23:13</t>
+          <t>06/05/2023 23:14</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-avai/xlW7DvM5/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-vila-nova-fc/YeZjHMMt/</t>
         </is>
       </c>
     </row>
@@ -4161,71 +4161,71 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="I41" t="n">
         <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>2.07</v>
+        <v>2.3</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>06/05/2023 15:09</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>06/05/2023 23:09</t>
+          <t>06/05/2023 23:13</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>3.06</v>
+        <v>3.08</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>06/05/2023 15:09</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>3.3</v>
+        <v>3.44</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>06/05/2023 23:10</t>
+          <t>06/05/2023 23:13</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>3.96</v>
+        <v>3.31</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>06/05/2023 15:09</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>4.55</v>
+        <v>4.11</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>06/05/2023 23:14</t>
+          <t>06/05/2023 23:13</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-vila-nova-fc/YeZjHMMt/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-esporte-clube-juventude/UNSaF0ig/</t>
         </is>
       </c>
     </row>
@@ -4253,30 +4253,30 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I42" t="n">
         <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -4284,15 +4284,15 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.08</v>
+        <v>3.21</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>3.44</v>
+        <v>3.32</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -4300,15 +4300,15 @@
         </is>
       </c>
       <c r="R42" t="n">
-        <v>3.31</v>
+        <v>3.4</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>4.11</v>
+        <v>4.16</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-esporte-clube-juventude/UNSaF0ig/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-avai/xlW7DvM5/</t>
         </is>
       </c>
     </row>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J64" t="n">
-        <v>1.93</v>
+        <v>2.65</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>14/05/2023 23:12</t>
+          <t>15/05/2023 01:42</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>1.91</v>
+        <v>2.71</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>20/05/2023 21:52</t>
+          <t>20/05/2023 21:59</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.34</v>
+        <v>3.13</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>14/05/2023 23:12</t>
+          <t>15/05/2023 01:42</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.47</v>
+        <v>3.08</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>20/05/2023 21:57</t>
+          <t>20/05/2023 21:59</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>4.4</v>
+        <v>2.75</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>14/05/2023 23:12</t>
+          <t>15/05/2023 01:42</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>4.47</v>
+        <v>2.94</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>20/05/2023 21:57</t>
+          <t>20/05/2023 21:50</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-abc/f77MOPo4/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-novorizontino/KlF9RR1o/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G65" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
         <v>0</v>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Novorizontino</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
-        <v>2</v>
-      </c>
       <c r="J65" t="n">
-        <v>2.65</v>
+        <v>1.93</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>15/05/2023 01:42</t>
+          <t>14/05/2023 23:12</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.71</v>
+        <v>1.91</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>20/05/2023 21:59</t>
+          <t>20/05/2023 21:52</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>3.13</v>
+        <v>3.34</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>15/05/2023 01:42</t>
+          <t>14/05/2023 23:12</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>3.08</v>
+        <v>3.47</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>20/05/2023 21:59</t>
+          <t>20/05/2023 21:57</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>2.75</v>
+        <v>4.4</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>15/05/2023 01:42</t>
+          <t>14/05/2023 23:12</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>2.94</v>
+        <v>4.47</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>20/05/2023 21:50</t>
+          <t>20/05/2023 21:57</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-novorizontino/KlF9RR1o/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-abc/f77MOPo4/</t>
         </is>
       </c>
     </row>
@@ -7197,71 +7197,71 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="I74" t="n">
         <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>1.84</v>
+        <v>2.5</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>21/05/2023 23:42</t>
+          <t>21/05/2023 16:12</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>1.77</v>
+        <v>2.15</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:56</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.32</v>
+        <v>3.12</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>21/05/2023 23:42</t>
+          <t>21/05/2023 16:12</t>
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.39</v>
+        <v>3.35</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:53</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>4.98</v>
+        <v>3.1</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>21/05/2023 23:42</t>
+          <t>21/05/2023 16:12</t>
         </is>
       </c>
       <c r="T74" t="n">
-        <v>5.65</v>
+        <v>3.7</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:56</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ituano/428cG1gp/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-atletico-go/ljr1zNpG/</t>
         </is>
       </c>
     </row>
@@ -7381,71 +7381,71 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="I76" t="n">
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>2.5</v>
+        <v>1.84</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>21/05/2023 16:12</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2.15</v>
+        <v>1.77</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:56</t>
         </is>
       </c>
       <c r="N76" t="n">
-        <v>3.12</v>
+        <v>3.32</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>21/05/2023 16:12</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="P76" t="n">
-        <v>3.35</v>
+        <v>3.39</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:53</t>
         </is>
       </c>
       <c r="R76" t="n">
-        <v>3.1</v>
+        <v>4.98</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>21/05/2023 16:12</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="T76" t="n">
-        <v>3.7</v>
+        <v>5.65</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:56</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-atletico-go/ljr1zNpG/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ituano/428cG1gp/</t>
         </is>
       </c>
     </row>
@@ -7565,71 +7565,71 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="I78" t="n">
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>2.31</v>
+        <v>2.28</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="L78" t="n">
-        <v>2.45</v>
+        <v>2.25</v>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:28</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="N78" t="n">
-        <v>3.17</v>
+        <v>3.09</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="P78" t="n">
-        <v>3.03</v>
+        <v>3.08</v>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:29</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="R78" t="n">
-        <v>3.21</v>
+        <v>3.35</v>
       </c>
       <c r="S78" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="T78" t="n">
-        <v>3.39</v>
+        <v>3.78</v>
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:28</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sport-recife/I5C1FL8j/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ponte-preta/6Rhdy3V9/</t>
         </is>
       </c>
     </row>
@@ -7657,71 +7657,71 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I79" t="n">
         <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>2.28</v>
+        <v>2.31</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:28</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>3.09</v>
+        <v>3.17</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="P79" t="n">
-        <v>3.08</v>
+        <v>3.03</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:29</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>3.35</v>
+        <v>3.21</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="T79" t="n">
-        <v>3.78</v>
+        <v>3.39</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:28</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ponte-preta/6Rhdy3V9/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sport-recife/I5C1FL8j/</t>
         </is>
       </c>
     </row>
@@ -8209,22 +8209,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J85" t="n">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2</v>
+        <v>2.09</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:20</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.36</v>
+        <v>3.22</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.31</v>
+        <v>3.18</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:29</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>4.05</v>
+        <v>3.8</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>4.3</v>
+        <v>4.15</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:29</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-criciuma/td9WxG6E/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-novorizontino/2BcuyfyR/</t>
         </is>
       </c>
     </row>
@@ -8301,22 +8301,22 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Criciuma</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
         <v>0</v>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Novorizontino</t>
-        </is>
-      </c>
-      <c r="I86" t="n">
-        <v>3</v>
-      </c>
       <c r="J86" t="n">
-        <v>2.05</v>
+        <v>2.04</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -8324,15 +8324,15 @@
         </is>
       </c>
       <c r="L86" t="n">
-        <v>2.09</v>
+        <v>2</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:20</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="N86" t="n">
-        <v>3.22</v>
+        <v>3.36</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -8340,15 +8340,15 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>3.18</v>
+        <v>3.31</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:29</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="R86" t="n">
-        <v>3.8</v>
+        <v>4.05</v>
       </c>
       <c r="S86" t="inlineStr">
         <is>
@@ -8356,16 +8356,16 @@
         </is>
       </c>
       <c r="T86" t="n">
-        <v>4.15</v>
+        <v>4.3</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:29</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-novorizontino/2BcuyfyR/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-criciuma/td9WxG6E/</t>
         </is>
       </c>
     </row>
@@ -8669,22 +8669,22 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="I90" t="n">
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>2.09</v>
+        <v>1.7</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>2.05</v>
+        <v>1.61</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:58</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.28</v>
+        <v>3.48</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.36</v>
+        <v>3.87</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:58</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>3.61</v>
+        <v>5.2</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>4.03</v>
+        <v>6.37</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:59</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-tombense/IsKAjZzE/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-chapecoense-sc/Qm9ppXDs/</t>
         </is>
       </c>
     </row>
@@ -8761,22 +8761,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="I91" t="n">
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>1.7</v>
+        <v>2.09</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>1.61</v>
+        <v>2.05</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:58</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>3.48</v>
+        <v>3.28</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>3.87</v>
+        <v>3.36</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:58</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>5.2</v>
+        <v>3.61</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>6.37</v>
+        <v>4.03</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:59</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-chapecoense-sc/Qm9ppXDs/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-tombense/IsKAjZzE/</t>
         </is>
       </c>
     </row>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -8861,14 +8861,14 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="I92" t="n">
         <v>0</v>
       </c>
       <c r="J92" t="n">
-        <v>2.06</v>
+        <v>1.69</v>
       </c>
       <c r="K92" t="inlineStr">
         <is>
@@ -8876,15 +8876,15 @@
         </is>
       </c>
       <c r="L92" t="n">
-        <v>2.11</v>
+        <v>1.78</v>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>03/06/2023 02:13</t>
+          <t>03/06/2023 02:24</t>
         </is>
       </c>
       <c r="N92" t="n">
-        <v>3.24</v>
+        <v>3.53</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
@@ -8892,15 +8892,15 @@
         </is>
       </c>
       <c r="P92" t="n">
-        <v>3.1</v>
+        <v>3.51</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>03/06/2023 02:13</t>
+          <t>03/06/2023 02:24</t>
         </is>
       </c>
       <c r="R92" t="n">
-        <v>3.73</v>
+        <v>5.21</v>
       </c>
       <c r="S92" t="inlineStr">
         <is>
@@ -8908,16 +8908,16 @@
         </is>
       </c>
       <c r="T92" t="n">
-        <v>4.21</v>
+        <v>5.29</v>
       </c>
       <c r="U92" t="inlineStr">
         <is>
-          <t>03/06/2023 02:13</t>
+          <t>03/06/2023 02:24</t>
         </is>
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-atletico-go/tQzSRkbD/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-ituano/jeIIlD5Q/</t>
         </is>
       </c>
     </row>
@@ -8945,7 +8945,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -8953,14 +8953,14 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="I93" t="n">
         <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.69</v>
+        <v>2.06</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -8968,15 +8968,15 @@
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.78</v>
+        <v>2.11</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>03/06/2023 02:24</t>
+          <t>03/06/2023 02:13</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.53</v>
+        <v>3.24</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -8984,15 +8984,15 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.51</v>
+        <v>3.1</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>03/06/2023 02:24</t>
+          <t>03/06/2023 02:13</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>5.21</v>
+        <v>3.73</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
@@ -9000,16 +9000,16 @@
         </is>
       </c>
       <c r="T93" t="n">
-        <v>5.29</v>
+        <v>4.21</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>03/06/2023 02:24</t>
+          <t>03/06/2023 02:13</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-ituano/jeIIlD5Q/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-atletico-go/tQzSRkbD/</t>
         </is>
       </c>
     </row>
@@ -9589,7 +9589,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -9597,63 +9597,63 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="I100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>1.7</v>
+        <v>2.37</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>03/06/2023 22:12</t>
+          <t>04/06/2023 00:13</t>
         </is>
       </c>
       <c r="L100" t="n">
-        <v>1.58</v>
+        <v>2.81</v>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>06/06/2023 23:38</t>
+          <t>06/06/2023 23:59</t>
         </is>
       </c>
       <c r="N100" t="n">
-        <v>3.56</v>
+        <v>3.05</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>03/06/2023 22:12</t>
+          <t>04/06/2023 00:13</t>
         </is>
       </c>
       <c r="P100" t="n">
-        <v>3.74</v>
+        <v>2.99</v>
       </c>
       <c r="Q100" t="inlineStr">
         <is>
-          <t>06/06/2023 23:38</t>
+          <t>06/06/2023 23:59</t>
         </is>
       </c>
       <c r="R100" t="n">
-        <v>5.08</v>
+        <v>3.22</v>
       </c>
       <c r="S100" t="inlineStr">
         <is>
-          <t>03/06/2023 22:12</t>
+          <t>04/06/2023 00:13</t>
         </is>
       </c>
       <c r="T100" t="n">
-        <v>7.21</v>
+        <v>2.92</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>06/06/2023 23:38</t>
+          <t>06/06/2023 23:59</t>
         </is>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-abc/fT01tkD6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-vila-nova-fc/6saOeUCg/</t>
         </is>
       </c>
     </row>
@@ -9681,30 +9681,30 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="G101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="I101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J101" t="n">
-        <v>2.37</v>
+        <v>2.46</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>04/06/2023 00:13</t>
+          <t>03/06/2023 02:42</t>
         </is>
       </c>
       <c r="L101" t="n">
-        <v>2.81</v>
+        <v>2.46</v>
       </c>
       <c r="M101" t="inlineStr">
         <is>
@@ -9712,15 +9712,15 @@
         </is>
       </c>
       <c r="N101" t="n">
-        <v>3.05</v>
+        <v>3.03</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>04/06/2023 00:13</t>
+          <t>03/06/2023 02:42</t>
         </is>
       </c>
       <c r="P101" t="n">
-        <v>2.99</v>
+        <v>3.18</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
@@ -9728,15 +9728,15 @@
         </is>
       </c>
       <c r="R101" t="n">
-        <v>3.22</v>
+        <v>3.08</v>
       </c>
       <c r="S101" t="inlineStr">
         <is>
-          <t>04/06/2023 00:13</t>
+          <t>03/06/2023 02:42</t>
         </is>
       </c>
       <c r="T101" t="n">
-        <v>2.92</v>
+        <v>3.2</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
@@ -9745,7 +9745,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-vila-nova-fc/6saOeUCg/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vitoria/Kp3SflSa/</t>
         </is>
       </c>
     </row>
@@ -9773,71 +9773,71 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="G102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J102" t="n">
-        <v>2.46</v>
+        <v>1.7</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>03/06/2023 02:42</t>
+          <t>03/06/2023 22:12</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.46</v>
+        <v>1.58</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>06/06/2023 23:59</t>
+          <t>06/06/2023 23:38</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.03</v>
+        <v>3.56</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>03/06/2023 02:42</t>
+          <t>03/06/2023 22:12</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.18</v>
+        <v>3.74</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>06/06/2023 23:59</t>
+          <t>06/06/2023 23:38</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>3.08</v>
+        <v>5.08</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>03/06/2023 02:42</t>
+          <t>03/06/2023 22:12</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>3.2</v>
+        <v>7.21</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>06/06/2023 23:59</t>
+          <t>06/06/2023 23:38</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vitoria/Kp3SflSa/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-abc/fT01tkD6/</t>
         </is>
       </c>
     </row>
@@ -16397,30 +16397,30 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="G174" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="I174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J174" t="n">
-        <v>1.45</v>
+        <v>2.28</v>
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>16/07/2023 23:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="L174" t="n">
-        <v>1.5</v>
+        <v>2.27</v>
       </c>
       <c r="M174" t="inlineStr">
         <is>
@@ -16428,40 +16428,40 @@
         </is>
       </c>
       <c r="N174" t="n">
-        <v>4.06</v>
+        <v>3.13</v>
       </c>
       <c r="O174" t="inlineStr">
         <is>
-          <t>16/07/2023 23:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="P174" t="n">
-        <v>4.02</v>
+        <v>3.12</v>
       </c>
       <c r="Q174" t="inlineStr">
         <is>
-          <t>19/07/2023 23:58</t>
+          <t>19/07/2023 23:57</t>
         </is>
       </c>
       <c r="R174" t="n">
-        <v>7.52</v>
+        <v>3.31</v>
       </c>
       <c r="S174" t="inlineStr">
         <is>
-          <t>16/07/2023 23:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="T174" t="n">
-        <v>8.199999999999999</v>
+        <v>3.67</v>
       </c>
       <c r="U174" t="inlineStr">
         <is>
-          <t>19/07/2023 23:58</t>
+          <t>19/07/2023 23:54</t>
         </is>
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-londrina/YkdOuXvn/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-mirassol/GYR9M9vO/</t>
         </is>
       </c>
     </row>
@@ -16489,30 +16489,30 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="G175" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="I175" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J175" t="n">
-        <v>2.28</v>
+        <v>1.45</v>
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>16/07/2023 23:12</t>
         </is>
       </c>
       <c r="L175" t="n">
-        <v>2.27</v>
+        <v>1.5</v>
       </c>
       <c r="M175" t="inlineStr">
         <is>
@@ -16520,40 +16520,40 @@
         </is>
       </c>
       <c r="N175" t="n">
-        <v>3.13</v>
+        <v>4.06</v>
       </c>
       <c r="O175" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>16/07/2023 23:12</t>
         </is>
       </c>
       <c r="P175" t="n">
-        <v>3.12</v>
+        <v>4.02</v>
       </c>
       <c r="Q175" t="inlineStr">
         <is>
-          <t>19/07/2023 23:57</t>
+          <t>19/07/2023 23:58</t>
         </is>
       </c>
       <c r="R175" t="n">
-        <v>3.31</v>
+        <v>7.52</v>
       </c>
       <c r="S175" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>16/07/2023 23:12</t>
         </is>
       </c>
       <c r="T175" t="n">
-        <v>3.67</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="U175" t="inlineStr">
         <is>
-          <t>19/07/2023 23:54</t>
+          <t>19/07/2023 23:58</t>
         </is>
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-mirassol/GYR9M9vO/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-londrina/YkdOuXvn/</t>
         </is>
       </c>
     </row>
@@ -16673,71 +16673,71 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="I177" t="n">
         <v>0</v>
       </c>
       <c r="J177" t="n">
-        <v>2.58</v>
+        <v>2.2</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="L177" t="n">
-        <v>2.69</v>
+        <v>2.05</v>
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>20/07/2023 02:25</t>
+          <t>20/07/2023 02:29</t>
         </is>
       </c>
       <c r="N177" t="n">
-        <v>2.99</v>
+        <v>3.05</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="P177" t="n">
-        <v>2.81</v>
+        <v>2.98</v>
       </c>
       <c r="Q177" t="inlineStr">
         <is>
-          <t>20/07/2023 02:25</t>
+          <t>20/07/2023 02:29</t>
         </is>
       </c>
       <c r="R177" t="n">
-        <v>2.95</v>
+        <v>3.82</v>
       </c>
       <c r="S177" t="inlineStr">
         <is>
-          <t>16/07/2023 20:42</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="T177" t="n">
-        <v>3.29</v>
+        <v>4.71</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
-          <t>20/07/2023 02:25</t>
+          <t>20/07/2023 02:29</t>
         </is>
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-vila-nova-fc/63fWwB9b/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-sampaio-correa/fPQDLTgU/</t>
         </is>
       </c>
     </row>
@@ -16765,30 +16765,30 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="I178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J178" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>15/07/2023 02:42</t>
+          <t>15/07/2023 16:12</t>
         </is>
       </c>
       <c r="L178" t="n">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="M178" t="inlineStr">
         <is>
@@ -16796,40 +16796,40 @@
         </is>
       </c>
       <c r="N178" t="n">
-        <v>3.05</v>
+        <v>2.85</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
-          <t>15/07/2023 02:42</t>
+          <t>15/07/2023 16:12</t>
         </is>
       </c>
       <c r="P178" t="n">
-        <v>2.98</v>
+        <v>2.81</v>
       </c>
       <c r="Q178" t="inlineStr">
         <is>
+          <t>20/07/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R178" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
+          <t>15/07/2023 16:12</t>
+        </is>
+      </c>
+      <c r="T178" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="U178" t="inlineStr">
+        <is>
           <t>20/07/2023 02:29</t>
         </is>
       </c>
-      <c r="R178" t="n">
-        <v>3.82</v>
-      </c>
-      <c r="S178" t="inlineStr">
-        <is>
-          <t>15/07/2023 02:42</t>
-        </is>
-      </c>
-      <c r="T178" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="U178" t="inlineStr">
-        <is>
-          <t>20/07/2023 02:29</t>
-        </is>
-      </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-sampaio-correa/fPQDLTgU/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-guarani/KS9yy9gH/</t>
         </is>
       </c>
     </row>
@@ -16857,42 +16857,42 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="G179" t="n">
+        <v>1</v>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Vila Nova FC</t>
+        </is>
+      </c>
+      <c r="I179" t="n">
         <v>0</v>
       </c>
-      <c r="H179" t="inlineStr">
-        <is>
-          <t>Guarani</t>
-        </is>
-      </c>
-      <c r="I179" t="n">
-        <v>1</v>
-      </c>
       <c r="J179" t="n">
-        <v>2.6</v>
+        <v>2.58</v>
       </c>
       <c r="K179" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="L179" t="n">
-        <v>2.6</v>
+        <v>2.69</v>
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>20/07/2023 02:29</t>
+          <t>20/07/2023 02:25</t>
         </is>
       </c>
       <c r="N179" t="n">
-        <v>2.85</v>
+        <v>2.99</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="P179" t="n">
@@ -16900,28 +16900,28 @@
       </c>
       <c r="Q179" t="inlineStr">
         <is>
-          <t>20/07/2023 02:26</t>
+          <t>20/07/2023 02:25</t>
         </is>
       </c>
       <c r="R179" t="n">
-        <v>3.08</v>
+        <v>2.95</v>
       </c>
       <c r="S179" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>16/07/2023 20:42</t>
         </is>
       </c>
       <c r="T179" t="n">
-        <v>3.42</v>
+        <v>3.29</v>
       </c>
       <c r="U179" t="inlineStr">
         <is>
-          <t>20/07/2023 02:29</t>
+          <t>20/07/2023 02:25</t>
         </is>
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-guarani/KS9yy9gH/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-vila-nova-fc/63fWwB9b/</t>
         </is>
       </c>
     </row>
@@ -18237,71 +18237,71 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="G194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="I194" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J194" t="n">
-        <v>2.05</v>
+        <v>2.23</v>
       </c>
       <c r="K194" t="inlineStr">
         <is>
-          <t>25/07/2023 00:12</t>
+          <t>23/07/2023 16:12</t>
         </is>
       </c>
       <c r="L194" t="n">
-        <v>2.18</v>
+        <v>2.4</v>
       </c>
       <c r="M194" t="inlineStr">
         <is>
-          <t>29/07/2023 21:51</t>
+          <t>29/07/2023 21:58</t>
         </is>
       </c>
       <c r="N194" t="n">
-        <v>3.05</v>
+        <v>3.02</v>
       </c>
       <c r="O194" t="inlineStr">
         <is>
-          <t>25/07/2023 00:12</t>
+          <t>23/07/2023 16:12</t>
         </is>
       </c>
       <c r="P194" t="n">
-        <v>3.07</v>
+        <v>2.86</v>
       </c>
       <c r="Q194" t="inlineStr">
         <is>
-          <t>29/07/2023 21:51</t>
+          <t>29/07/2023 21:57</t>
         </is>
       </c>
       <c r="R194" t="n">
-        <v>4.35</v>
+        <v>3.78</v>
       </c>
       <c r="S194" t="inlineStr">
         <is>
-          <t>25/07/2023 00:12</t>
+          <t>23/07/2023 16:12</t>
         </is>
       </c>
       <c r="T194" t="n">
-        <v>4.02</v>
+        <v>3.74</v>
       </c>
       <c r="U194" t="inlineStr">
         <is>
-          <t>29/07/2023 21:51</t>
+          <t>29/07/2023 21:58</t>
         </is>
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-londrina/rq200PMS/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-guarani/QsYhspGj/</t>
         </is>
       </c>
     </row>
@@ -18329,71 +18329,71 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="I195" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J195" t="n">
-        <v>2.23</v>
+        <v>2.05</v>
       </c>
       <c r="K195" t="inlineStr">
         <is>
-          <t>23/07/2023 16:12</t>
+          <t>25/07/2023 00:12</t>
         </is>
       </c>
       <c r="L195" t="n">
-        <v>2.4</v>
+        <v>2.18</v>
       </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>29/07/2023 21:58</t>
+          <t>29/07/2023 21:51</t>
         </is>
       </c>
       <c r="N195" t="n">
-        <v>3.02</v>
+        <v>3.05</v>
       </c>
       <c r="O195" t="inlineStr">
         <is>
-          <t>23/07/2023 16:12</t>
+          <t>25/07/2023 00:12</t>
         </is>
       </c>
       <c r="P195" t="n">
-        <v>2.86</v>
+        <v>3.07</v>
       </c>
       <c r="Q195" t="inlineStr">
         <is>
-          <t>29/07/2023 21:57</t>
+          <t>29/07/2023 21:51</t>
         </is>
       </c>
       <c r="R195" t="n">
-        <v>3.78</v>
+        <v>4.35</v>
       </c>
       <c r="S195" t="inlineStr">
         <is>
-          <t>23/07/2023 16:12</t>
+          <t>25/07/2023 00:12</t>
         </is>
       </c>
       <c r="T195" t="n">
-        <v>3.74</v>
+        <v>4.02</v>
       </c>
       <c r="U195" t="inlineStr">
         <is>
-          <t>29/07/2023 21:58</t>
+          <t>29/07/2023 21:51</t>
         </is>
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-guarani/QsYhspGj/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-londrina/rq200PMS/</t>
         </is>
       </c>
     </row>
@@ -18789,46 +18789,46 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G200" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I200" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J200" t="n">
-        <v>1.57</v>
+        <v>2.02</v>
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="L200" t="n">
-        <v>1.66</v>
+        <v>2.09</v>
       </c>
       <c r="M200" t="inlineStr">
         <is>
-          <t>01/08/2023 23:33</t>
+          <t>01/08/2023 23:51</t>
         </is>
       </c>
       <c r="N200" t="n">
-        <v>3.79</v>
+        <v>3.06</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="P200" t="n">
-        <v>3.68</v>
+        <v>3.06</v>
       </c>
       <c r="Q200" t="inlineStr">
         <is>
@@ -18836,24 +18836,24 @@
         </is>
       </c>
       <c r="R200" t="n">
-        <v>6.77</v>
+        <v>4.16</v>
       </c>
       <c r="S200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="T200" t="n">
-        <v>6.16</v>
+        <v>4.39</v>
       </c>
       <c r="U200" t="inlineStr">
         <is>
-          <t>01/08/2023 23:33</t>
+          <t>01/08/2023 23:51</t>
         </is>
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-avai/6cZMHQi3/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-botafogo-sp/SCNVF4MF/</t>
         </is>
       </c>
     </row>
@@ -18881,71 +18881,71 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J201" t="n">
-        <v>2.02</v>
+        <v>1.57</v>
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>29/07/2023 23:12</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="L201" t="n">
-        <v>2.09</v>
+        <v>1.66</v>
       </c>
       <c r="M201" t="inlineStr">
         <is>
+          <t>01/08/2023 23:33</t>
+        </is>
+      </c>
+      <c r="N201" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>29/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P201" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
           <t>01/08/2023 23:51</t>
         </is>
       </c>
-      <c r="N201" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="O201" t="inlineStr">
-        <is>
-          <t>29/07/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P201" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="Q201" t="inlineStr">
-        <is>
-          <t>01/08/2023 23:51</t>
-        </is>
-      </c>
       <c r="R201" t="n">
-        <v>4.16</v>
+        <v>6.77</v>
       </c>
       <c r="S201" t="inlineStr">
         <is>
-          <t>29/07/2023 23:12</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="T201" t="n">
-        <v>4.39</v>
+        <v>6.16</v>
       </c>
       <c r="U201" t="inlineStr">
         <is>
-          <t>01/08/2023 23:51</t>
+          <t>01/08/2023 23:33</t>
         </is>
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-botafogo-sp/SCNVF4MF/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-avai/6cZMHQi3/</t>
         </is>
       </c>
     </row>
@@ -19249,42 +19249,42 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="G205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="I205" t="n">
         <v>1</v>
       </c>
       <c r="J205" t="n">
-        <v>2.3</v>
+        <v>2.51</v>
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="L205" t="n">
-        <v>2.31</v>
+        <v>2.59</v>
       </c>
       <c r="M205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:19</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="N205" t="n">
-        <v>2.97</v>
+        <v>2.96</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="P205" t="n">
@@ -19292,28 +19292,28 @@
       </c>
       <c r="Q205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:19</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="R205" t="n">
-        <v>3.68</v>
+        <v>3.26</v>
       </c>
       <c r="S205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="T205" t="n">
-        <v>3.9</v>
+        <v>3.31</v>
       </c>
       <c r="U205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:27</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-sport-recife/2TrXf3pj/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-chapecoense-sc/YBk3cd6l/</t>
         </is>
       </c>
     </row>
@@ -19341,22 +19341,22 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="G206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J206" t="n">
-        <v>2.51</v>
+        <v>2.2</v>
       </c>
       <c r="K206" t="inlineStr">
         <is>
@@ -19364,15 +19364,15 @@
         </is>
       </c>
       <c r="L206" t="n">
-        <v>2.59</v>
+        <v>2.1</v>
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:28</t>
         </is>
       </c>
       <c r="N206" t="n">
-        <v>2.96</v>
+        <v>3.08</v>
       </c>
       <c r="O206" t="inlineStr">
         <is>
@@ -19380,15 +19380,15 @@
         </is>
       </c>
       <c r="P206" t="n">
-        <v>2.9</v>
+        <v>3.18</v>
       </c>
       <c r="Q206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:24</t>
         </is>
       </c>
       <c r="R206" t="n">
-        <v>3.26</v>
+        <v>3.79</v>
       </c>
       <c r="S206" t="inlineStr">
         <is>
@@ -19396,16 +19396,16 @@
         </is>
       </c>
       <c r="T206" t="n">
-        <v>3.31</v>
+        <v>4.11</v>
       </c>
       <c r="U206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:28</t>
         </is>
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-chapecoense-sc/YBk3cd6l/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-ceara/phlSeqVq/</t>
         </is>
       </c>
     </row>
@@ -19433,71 +19433,71 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="G207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I207" t="n">
         <v>0</v>
       </c>
       <c r="J207" t="n">
-        <v>2.2</v>
+        <v>2.38</v>
       </c>
       <c r="K207" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="L207" t="n">
-        <v>2.1</v>
+        <v>2.46</v>
       </c>
       <c r="M207" t="inlineStr">
         <is>
+          <t>03/08/2023 02:21</t>
+        </is>
+      </c>
+      <c r="N207" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="O207" t="inlineStr">
+        <is>
+          <t>30/07/2023 20:42</t>
+        </is>
+      </c>
+      <c r="P207" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="Q207" t="inlineStr">
+        <is>
           <t>03/08/2023 02:28</t>
         </is>
       </c>
-      <c r="N207" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="O207" t="inlineStr">
-        <is>
-          <t>29/07/2023 22:12</t>
-        </is>
-      </c>
-      <c r="P207" t="n">
-        <v>3.18</v>
-      </c>
-      <c r="Q207" t="inlineStr">
-        <is>
-          <t>03/08/2023 02:24</t>
-        </is>
-      </c>
       <c r="R207" t="n">
-        <v>3.79</v>
+        <v>3.51</v>
       </c>
       <c r="S207" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="T207" t="n">
-        <v>4.11</v>
+        <v>3.48</v>
       </c>
       <c r="U207" t="inlineStr">
         <is>
-          <t>03/08/2023 02:28</t>
+          <t>03/08/2023 02:21</t>
         </is>
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-ceara/phlSeqVq/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-novorizontino/fLjabxir/</t>
         </is>
       </c>
     </row>
@@ -19525,71 +19525,71 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G208" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I208" t="n">
         <v>0</v>
       </c>
       <c r="J208" t="n">
-        <v>2.38</v>
+        <v>1.6</v>
       </c>
       <c r="K208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="L208" t="n">
-        <v>2.46</v>
+        <v>1.47</v>
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:21</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="N208" t="n">
-        <v>2.96</v>
+        <v>3.78</v>
       </c>
       <c r="O208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="P208" t="n">
-        <v>2.94</v>
+        <v>4.23</v>
       </c>
       <c r="Q208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:28</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="R208" t="n">
-        <v>3.51</v>
+        <v>5.67</v>
       </c>
       <c r="S208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="T208" t="n">
-        <v>3.48</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="U208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:21</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-novorizontino/fLjabxir/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-abc/lMORGp79/</t>
         </is>
       </c>
     </row>
@@ -19617,71 +19617,71 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G209" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J209" t="n">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="L209" t="n">
-        <v>1.47</v>
+        <v>2.31</v>
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:19</t>
         </is>
       </c>
       <c r="N209" t="n">
-        <v>3.78</v>
+        <v>2.97</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="P209" t="n">
-        <v>4.23</v>
+        <v>2.9</v>
       </c>
       <c r="Q209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:19</t>
         </is>
       </c>
       <c r="R209" t="n">
-        <v>5.67</v>
+        <v>3.68</v>
       </c>
       <c r="S209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="T209" t="n">
-        <v>8.199999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="U209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:27</t>
         </is>
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-abc/lMORGp79/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-sport-recife/2TrXf3pj/</t>
         </is>
       </c>
     </row>
@@ -19893,71 +19893,71 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="I212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J212" t="n">
-        <v>1.98</v>
+        <v>2.48</v>
       </c>
       <c r="K212" t="inlineStr">
         <is>
-          <t>02/08/2023 02:41</t>
+          <t>03/08/2023 02:42</t>
         </is>
       </c>
       <c r="L212" t="n">
-        <v>1.78</v>
+        <v>2.77</v>
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>05/08/2023 21:56</t>
+          <t>05/08/2023 21:50</t>
         </is>
       </c>
       <c r="N212" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="O212" t="inlineStr">
         <is>
-          <t>02/08/2023 02:41</t>
+          <t>03/08/2023 02:42</t>
         </is>
       </c>
       <c r="P212" t="n">
-        <v>3.4</v>
+        <v>2.83</v>
       </c>
       <c r="Q212" t="inlineStr">
         <is>
-          <t>05/08/2023 21:56</t>
+          <t>05/08/2023 21:50</t>
         </is>
       </c>
       <c r="R212" t="n">
-        <v>4.54</v>
+        <v>3.02</v>
       </c>
       <c r="S212" t="inlineStr">
         <is>
-          <t>02/08/2023 02:41</t>
+          <t>03/08/2023 02:42</t>
         </is>
       </c>
       <c r="T212" t="n">
-        <v>5.51</v>
+        <v>3.15</v>
       </c>
       <c r="U212" t="inlineStr">
         <is>
-          <t>05/08/2023 21:55</t>
+          <t>05/08/2023 21:57</t>
         </is>
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-botafogo-sp/lIps9g50/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-guarani/lf2fIcrE/</t>
         </is>
       </c>
     </row>
@@ -19985,71 +19985,71 @@
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J213" t="n">
-        <v>2.48</v>
+        <v>1.98</v>
       </c>
       <c r="K213" t="inlineStr">
         <is>
-          <t>03/08/2023 02:42</t>
+          <t>02/08/2023 02:41</t>
         </is>
       </c>
       <c r="L213" t="n">
-        <v>2.77</v>
+        <v>1.78</v>
       </c>
       <c r="M213" t="inlineStr">
         <is>
-          <t>05/08/2023 21:50</t>
+          <t>05/08/2023 21:56</t>
         </is>
       </c>
       <c r="N213" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="O213" t="inlineStr">
         <is>
-          <t>03/08/2023 02:42</t>
+          <t>02/08/2023 02:41</t>
         </is>
       </c>
       <c r="P213" t="n">
-        <v>2.83</v>
+        <v>3.4</v>
       </c>
       <c r="Q213" t="inlineStr">
         <is>
-          <t>05/08/2023 21:50</t>
+          <t>05/08/2023 21:56</t>
         </is>
       </c>
       <c r="R213" t="n">
-        <v>3.02</v>
+        <v>4.54</v>
       </c>
       <c r="S213" t="inlineStr">
         <is>
-          <t>03/08/2023 02:42</t>
+          <t>02/08/2023 02:41</t>
         </is>
       </c>
       <c r="T213" t="n">
-        <v>3.15</v>
+        <v>5.51</v>
       </c>
       <c r="U213" t="inlineStr">
         <is>
-          <t>05/08/2023 21:57</t>
+          <t>05/08/2023 21:55</t>
         </is>
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-guarani/lf2fIcrE/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-botafogo-sp/lIps9g50/</t>
         </is>
       </c>
     </row>
@@ -22009,22 +22009,22 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G235" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="I235" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J235" t="n">
-        <v>2.69</v>
+        <v>2.62</v>
       </c>
       <c r="K235" t="inlineStr">
         <is>
@@ -22032,7 +22032,7 @@
         </is>
       </c>
       <c r="L235" t="n">
-        <v>2.79</v>
+        <v>2.94</v>
       </c>
       <c r="M235" t="inlineStr">
         <is>
@@ -22040,7 +22040,7 @@
         </is>
       </c>
       <c r="N235" t="n">
-        <v>3</v>
+        <v>2.95</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -22048,32 +22048,32 @@
         </is>
       </c>
       <c r="P235" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>19/08/2023 21:57</t>
+        </is>
+      </c>
+      <c r="R235" t="n">
         <v>2.95</v>
       </c>
-      <c r="Q235" t="inlineStr">
+      <c r="S235" t="inlineStr">
+        <is>
+          <t>15/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T235" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="U235" t="inlineStr">
         <is>
           <t>19/08/2023 21:51</t>
         </is>
       </c>
-      <c r="R235" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="S235" t="inlineStr">
-        <is>
-          <t>15/08/2023 00:12</t>
-        </is>
-      </c>
-      <c r="T235" t="n">
-        <v>2.98</v>
-      </c>
-      <c r="U235" t="inlineStr">
-        <is>
-          <t>19/08/2023 21:51</t>
-        </is>
-      </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-criciuma/jmzKsEBP/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-crb/jBI6Y9YB/</t>
         </is>
       </c>
     </row>
@@ -22101,22 +22101,22 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G236" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="I236" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>2.62</v>
+        <v>2.69</v>
       </c>
       <c r="K236" t="inlineStr">
         <is>
@@ -22124,7 +22124,7 @@
         </is>
       </c>
       <c r="L236" t="n">
-        <v>2.94</v>
+        <v>2.79</v>
       </c>
       <c r="M236" t="inlineStr">
         <is>
@@ -22132,31 +22132,31 @@
         </is>
       </c>
       <c r="N236" t="n">
+        <v>3</v>
+      </c>
+      <c r="O236" t="inlineStr">
+        <is>
+          <t>15/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P236" t="n">
         <v>2.95</v>
       </c>
-      <c r="O236" t="inlineStr">
+      <c r="Q236" t="inlineStr">
+        <is>
+          <t>19/08/2023 21:51</t>
+        </is>
+      </c>
+      <c r="R236" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="S236" t="inlineStr">
         <is>
           <t>15/08/2023 00:12</t>
         </is>
       </c>
-      <c r="P236" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="Q236" t="inlineStr">
-        <is>
-          <t>19/08/2023 21:57</t>
-        </is>
-      </c>
-      <c r="R236" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="S236" t="inlineStr">
-        <is>
-          <t>15/08/2023 00:12</t>
-        </is>
-      </c>
       <c r="T236" t="n">
-        <v>2.99</v>
+        <v>2.98</v>
       </c>
       <c r="U236" t="inlineStr">
         <is>
@@ -22165,7 +22165,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-crb/jBI6Y9YB/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-criciuma/jmzKsEBP/</t>
         </is>
       </c>
     </row>
@@ -28633,22 +28633,22 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G307" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I307" t="n">
         <v>1</v>
       </c>
       <c r="J307" t="n">
-        <v>3.32</v>
+        <v>2.02</v>
       </c>
       <c r="K307" t="inlineStr">
         <is>
@@ -28656,15 +28656,15 @@
         </is>
       </c>
       <c r="L307" t="n">
-        <v>3.03</v>
+        <v>2.05</v>
       </c>
       <c r="M307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:59</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="N307" t="n">
-        <v>2.94</v>
+        <v>3.01</v>
       </c>
       <c r="O307" t="inlineStr">
         <is>
@@ -28672,15 +28672,15 @@
         </is>
       </c>
       <c r="P307" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="Q307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:51</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="R307" t="n">
-        <v>2.39</v>
+        <v>4.62</v>
       </c>
       <c r="S307" t="inlineStr">
         <is>
@@ -28688,16 +28688,16 @@
         </is>
       </c>
       <c r="T307" t="n">
-        <v>2.8</v>
+        <v>4.58</v>
       </c>
       <c r="U307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:59</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="V307" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-novorizontino/S4ibIC04/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-avai/hnaoLEGo/</t>
         </is>
       </c>
     </row>
@@ -28725,22 +28725,22 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I308" t="n">
         <v>1</v>
       </c>
       <c r="J308" t="n">
-        <v>2.02</v>
+        <v>3.32</v>
       </c>
       <c r="K308" t="inlineStr">
         <is>
@@ -28748,15 +28748,15 @@
         </is>
       </c>
       <c r="L308" t="n">
-        <v>2.05</v>
+        <v>3.03</v>
       </c>
       <c r="M308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:59</t>
         </is>
       </c>
       <c r="N308" t="n">
-        <v>3.01</v>
+        <v>2.94</v>
       </c>
       <c r="O308" t="inlineStr">
         <is>
@@ -28764,15 +28764,15 @@
         </is>
       </c>
       <c r="P308" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="Q308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:51</t>
         </is>
       </c>
       <c r="R308" t="n">
-        <v>4.62</v>
+        <v>2.39</v>
       </c>
       <c r="S308" t="inlineStr">
         <is>
@@ -28780,16 +28780,16 @@
         </is>
       </c>
       <c r="T308" t="n">
-        <v>4.58</v>
+        <v>2.8</v>
       </c>
       <c r="U308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:59</t>
         </is>
       </c>
       <c r="V308" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-avai/hnaoLEGo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-novorizontino/S4ibIC04/</t>
         </is>
       </c>
     </row>
@@ -31117,71 +31117,71 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="G334" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J334" t="n">
-        <v>1.53</v>
+        <v>1.64</v>
       </c>
       <c r="K334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="L334" t="n">
-        <v>1.39</v>
+        <v>1.7</v>
       </c>
       <c r="M334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:21</t>
+          <t>28/10/2023 02:05</t>
         </is>
       </c>
       <c r="N334" t="n">
-        <v>3.81</v>
+        <v>3.41</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="P334" t="n">
-        <v>4.57</v>
+        <v>3.43</v>
       </c>
       <c r="Q334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:28</t>
+          <t>28/10/2023 02:17</t>
         </is>
       </c>
       <c r="R334" t="n">
-        <v>6.57</v>
+        <v>6.14</v>
       </c>
       <c r="S334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="T334" t="n">
-        <v>10.13</v>
+        <v>6.36</v>
       </c>
       <c r="U334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:28</t>
+          <t>28/10/2023 02:24</t>
         </is>
       </c>
       <c r="V334" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-ponte-preta/EeWldSr9/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-botafogo-sp/QZkfzoMk/</t>
         </is>
       </c>
     </row>
@@ -31209,71 +31209,71 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="G335" t="n">
+        <v>2</v>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>Ponte Preta</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
         <v>0</v>
       </c>
-      <c r="H335" t="inlineStr">
-        <is>
-          <t>Botafogo SP</t>
-        </is>
-      </c>
-      <c r="I335" t="n">
-        <v>1</v>
-      </c>
       <c r="J335" t="n">
-        <v>1.64</v>
+        <v>1.53</v>
       </c>
       <c r="K335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="L335" t="n">
-        <v>1.7</v>
+        <v>1.39</v>
       </c>
       <c r="M335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:05</t>
+          <t>28/10/2023 02:21</t>
         </is>
       </c>
       <c r="N335" t="n">
-        <v>3.41</v>
+        <v>3.81</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="P335" t="n">
-        <v>3.43</v>
+        <v>4.57</v>
       </c>
       <c r="Q335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:17</t>
+          <t>28/10/2023 02:28</t>
         </is>
       </c>
       <c r="R335" t="n">
-        <v>6.14</v>
+        <v>6.57</v>
       </c>
       <c r="S335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="T335" t="n">
-        <v>6.36</v>
+        <v>10.13</v>
       </c>
       <c r="U335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:24</t>
+          <t>28/10/2023 02:28</t>
         </is>
       </c>
       <c r="V335" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-botafogo-sp/QZkfzoMk/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-ponte-preta/EeWldSr9/</t>
         </is>
       </c>
     </row>
@@ -31301,71 +31301,71 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G336" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H336" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="I336" t="n">
         <v>0</v>
       </c>
       <c r="J336" t="n">
-        <v>3.08</v>
+        <v>1.7</v>
       </c>
       <c r="K336" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 23:42</t>
         </is>
       </c>
       <c r="L336" t="n">
-        <v>3.71</v>
+        <v>1.58</v>
       </c>
       <c r="M336" t="inlineStr">
         <is>
-          <t>28/10/2023 20:24</t>
+          <t>28/10/2023 20:26</t>
         </is>
       </c>
       <c r="N336" t="n">
-        <v>2.89</v>
+        <v>3.42</v>
       </c>
       <c r="O336" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 23:42</t>
         </is>
       </c>
       <c r="P336" t="n">
-        <v>2.9</v>
+        <v>3.72</v>
       </c>
       <c r="Q336" t="inlineStr">
         <is>
-          <t>28/10/2023 20:24</t>
+          <t>28/10/2023 20:26</t>
         </is>
       </c>
       <c r="R336" t="n">
-        <v>2.57</v>
+        <v>5.95</v>
       </c>
       <c r="S336" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 23:42</t>
         </is>
       </c>
       <c r="T336" t="n">
-        <v>2.39</v>
+        <v>7.22</v>
       </c>
       <c r="U336" t="inlineStr">
         <is>
-          <t>28/10/2023 20:24</t>
+          <t>28/10/2023 20:26</t>
         </is>
       </c>
       <c r="V336" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-mirassol/z5Xpc8T2/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sampaio-correa/bml2YOj2/</t>
         </is>
       </c>
     </row>
@@ -31393,71 +31393,71 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G337" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H337" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="I337" t="n">
         <v>0</v>
       </c>
       <c r="J337" t="n">
-        <v>1.7</v>
+        <v>3.08</v>
       </c>
       <c r="K337" t="inlineStr">
         <is>
-          <t>21/10/2023 23:42</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="L337" t="n">
-        <v>1.58</v>
+        <v>3.71</v>
       </c>
       <c r="M337" t="inlineStr">
         <is>
-          <t>28/10/2023 20:26</t>
+          <t>28/10/2023 20:24</t>
         </is>
       </c>
       <c r="N337" t="n">
-        <v>3.42</v>
+        <v>2.89</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
-          <t>21/10/2023 23:42</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="P337" t="n">
-        <v>3.72</v>
+        <v>2.9</v>
       </c>
       <c r="Q337" t="inlineStr">
         <is>
-          <t>28/10/2023 20:26</t>
+          <t>28/10/2023 20:24</t>
         </is>
       </c>
       <c r="R337" t="n">
-        <v>5.95</v>
+        <v>2.57</v>
       </c>
       <c r="S337" t="inlineStr">
         <is>
-          <t>21/10/2023 23:42</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="T337" t="n">
-        <v>7.22</v>
+        <v>2.39</v>
       </c>
       <c r="U337" t="inlineStr">
         <is>
-          <t>28/10/2023 20:26</t>
+          <t>28/10/2023 20:24</t>
         </is>
       </c>
       <c r="V337" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sampaio-correa/bml2YOj2/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-mirassol/z5Xpc8T2/</t>
         </is>
       </c>
     </row>
@@ -32562,6 +32562,190 @@
       <c r="V349" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-vila-nova-fc/dt90iwcs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>serie-b</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E350" s="2" t="n">
+        <v>45237.95833333334</v>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>CRB</t>
+        </is>
+      </c>
+      <c r="G350" t="n">
+        <v>3</v>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>Chapecoense-SC</t>
+        </is>
+      </c>
+      <c r="I350" t="n">
+        <v>2</v>
+      </c>
+      <c r="J350" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="K350" t="inlineStr">
+        <is>
+          <t>01/11/2023 10:43</t>
+        </is>
+      </c>
+      <c r="L350" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="M350" t="inlineStr">
+        <is>
+          <t>07/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="N350" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="O350" t="inlineStr">
+        <is>
+          <t>01/11/2023 10:43</t>
+        </is>
+      </c>
+      <c r="P350" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="Q350" t="inlineStr">
+        <is>
+          <t>07/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="R350" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="S350" t="inlineStr">
+        <is>
+          <t>01/11/2023 10:43</t>
+        </is>
+      </c>
+      <c r="T350" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="U350" t="inlineStr">
+        <is>
+          <t>07/11/2023 22:58</t>
+        </is>
+      </c>
+      <c r="V350" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-chapecoense-sc/A3FGmed6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>serie-b</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E351" s="2" t="n">
+        <v>45238.0625</v>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>Criciuma</t>
+        </is>
+      </c>
+      <c r="G351" t="n">
+        <v>1</v>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="I351" t="n">
+        <v>0</v>
+      </c>
+      <c r="J351" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="K351" t="inlineStr">
+        <is>
+          <t>04/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="L351" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M351" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="N351" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="O351" t="inlineStr">
+        <is>
+          <t>04/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="P351" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="Q351" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="R351" t="n">
+        <v>8.57</v>
+      </c>
+      <c r="S351" t="inlineStr">
+        <is>
+          <t>04/11/2023 02:42</t>
+        </is>
+      </c>
+      <c r="T351" t="n">
+        <v>12.89</v>
+      </c>
+      <c r="U351" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="V351" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-abc/OhvnYFdJ/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 15-11-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/brazil_serie-b_2023.xlsx
+++ b/2023/brazil_serie-b_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V359"/>
+  <dimension ref="A1:V361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2229,46 +2229,46 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1.73</v>
+        <v>2.13</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>22/04/2023 21:12</t>
+          <t>23/04/2023 23:12</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>1.76</v>
+        <v>1.84</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>28/04/2023 23:49</t>
+          <t>28/04/2023 23:59</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.37</v>
+        <v>3.31</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>22/04/2023 21:12</t>
+          <t>23/04/2023 23:12</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.49</v>
+        <v>3.45</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
@@ -2276,15 +2276,15 @@
         </is>
       </c>
       <c r="R20" t="n">
-        <v>5.21</v>
+        <v>3.45</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>22/04/2023 21:12</t>
+          <t>23/04/2023 23:12</t>
         </is>
       </c>
       <c r="T20" t="n">
-        <v>5.46</v>
+        <v>4.94</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-avai/xd4Opkn2/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-londrina/W80E7CgF/</t>
         </is>
       </c>
     </row>
@@ -2321,71 +2321,71 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>2.13</v>
+        <v>1.73</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>23/04/2023 23:12</t>
+          <t>22/04/2023 21:12</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>1.84</v>
+        <v>1.76</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
+          <t>28/04/2023 23:49</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>22/04/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
           <t>28/04/2023 23:59</t>
         </is>
       </c>
-      <c r="N21" t="n">
-        <v>3.31</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>23/04/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P21" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="Q21" t="inlineStr">
+      <c r="R21" t="n">
+        <v>5.21</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>22/04/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T21" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="U21" t="inlineStr">
         <is>
           <t>28/04/2023 23:59</t>
         </is>
       </c>
-      <c r="R21" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>23/04/2023 23:12</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v>4.94</v>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>28/04/2023 23:59</t>
-        </is>
-      </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-londrina/W80E7CgF/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-avai/xd4Opkn2/</t>
         </is>
       </c>
     </row>
@@ -2597,19 +2597,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
         <v>2.2</v>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>2.43</v>
+        <v>2.37</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:57</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.09</v>
+        <v>3.04</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3</v>
+        <v>3.05</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:51</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.54</v>
+        <v>3.84</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>3.46</v>
+        <v>3.52</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>29/04/2023 21:57</t>
+          <t>29/04/2023 21:59</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-crb/jah69YO2/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ponte-preta/vZ3M5jOR/</t>
         </is>
       </c>
     </row>
@@ -2689,19 +2689,19 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>2.2</v>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>2.37</v>
+        <v>2.43</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:57</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>3.04</v>
+        <v>3.09</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:51</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>3.84</v>
+        <v>3.54</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>3.52</v>
+        <v>3.46</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>29/04/2023 21:59</t>
+          <t>29/04/2023 21:57</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ponte-preta/vZ3M5jOR/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-crb/jah69YO2/</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1.92</v>
+        <v>2.15</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.86</v>
+        <v>2.03</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:59</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.33</v>
+        <v>3.06</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,15 +3280,15 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.51</v>
+        <v>3.25</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:57</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>4.47</v>
+        <v>3.72</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,16 +3296,16 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>4.68</v>
+        <v>4.28</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>02/05/2023 23:59</t>
+          <t>02/05/2023 23:23</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-sampaio-correa/pf7UaLi6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-botafogo-sp/xAqcal1e/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>2.15</v>
+        <v>1.92</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.03</v>
+        <v>1.86</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:59</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.06</v>
+        <v>3.33</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3372,15 +3372,15 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>3.25</v>
+        <v>3.51</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:57</t>
         </is>
       </c>
       <c r="R32" t="n">
-        <v>3.72</v>
+        <v>4.47</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -3388,16 +3388,16 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>4.28</v>
+        <v>4.68</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>02/05/2023 23:23</t>
+          <t>02/05/2023 23:59</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-botafogo-sp/xAqcal1e/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-sampaio-correa/pf7UaLi6/</t>
         </is>
       </c>
     </row>
@@ -3517,46 +3517,46 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
         <v>0</v>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Novorizontino</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>2</v>
-      </c>
       <c r="J34" t="n">
-        <v>2.25</v>
+        <v>1.88</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>30/04/2023 20:42</t>
+          <t>30/04/2023 23:13</t>
         </is>
       </c>
       <c r="L34" t="n">
-        <v>2.27</v>
+        <v>2.3</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>03/05/2023 23:59</t>
+          <t>03/05/2023 23:57</t>
         </is>
       </c>
       <c r="N34" t="n">
-        <v>3.15</v>
+        <v>3.35</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>30/04/2023 20:42</t>
+          <t>30/04/2023 23:13</t>
         </is>
       </c>
       <c r="P34" t="n">
-        <v>3.13</v>
+        <v>3.09</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -3564,24 +3564,24 @@
         </is>
       </c>
       <c r="R34" t="n">
-        <v>3.35</v>
+        <v>4.28</v>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>30/04/2023 20:42</t>
+          <t>30/04/2023 23:13</t>
         </is>
       </c>
       <c r="T34" t="n">
-        <v>3.65</v>
+        <v>3.63</v>
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>03/05/2023 23:59</t>
+          <t>03/05/2023 23:57</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-novorizontino/l6npLVNE/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-abc/AFmtMB88/</t>
         </is>
       </c>
     </row>
@@ -3609,71 +3609,71 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35" t="n">
-        <v>1.88</v>
+        <v>2.25</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>30/04/2023 23:13</t>
+          <t>30/04/2023 20:42</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>2.3</v>
+        <v>2.27</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
+          <t>03/05/2023 23:59</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>30/04/2023 20:42</t>
+        </is>
+      </c>
+      <c r="P35" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
           <t>03/05/2023 23:57</t>
         </is>
       </c>
-      <c r="N35" t="n">
+      <c r="R35" t="n">
         <v>3.35</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>30/04/2023 23:13</t>
-        </is>
-      </c>
-      <c r="P35" t="n">
-        <v>3.09</v>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>03/05/2023 23:57</t>
-        </is>
-      </c>
-      <c r="R35" t="n">
-        <v>4.28</v>
-      </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>30/04/2023 23:13</t>
+          <t>30/04/2023 20:42</t>
         </is>
       </c>
       <c r="T35" t="n">
-        <v>3.63</v>
+        <v>3.65</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>03/05/2023 23:57</t>
+          <t>03/05/2023 23:59</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-abc/AFmtMB88/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-novorizontino/l6npLVNE/</t>
         </is>
       </c>
     </row>
@@ -4069,30 +4069,30 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I40" t="n">
         <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="L40" t="n">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
@@ -4100,15 +4100,15 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>3.08</v>
+        <v>3.21</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="P40" t="n">
-        <v>3.44</v>
+        <v>3.32</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
@@ -4116,15 +4116,15 @@
         </is>
       </c>
       <c r="R40" t="n">
-        <v>3.31</v>
+        <v>3.4</v>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>04/05/2023 00:12</t>
+          <t>04/05/2023 02:42</t>
         </is>
       </c>
       <c r="T40" t="n">
-        <v>4.11</v>
+        <v>4.16</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
@@ -4133,7 +4133,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-esporte-clube-juventude/UNSaF0ig/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-avai/xlW7DvM5/</t>
         </is>
       </c>
     </row>
@@ -4253,30 +4253,30 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="I42" t="n">
         <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>2.03</v>
+        <v>2</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -4284,15 +4284,15 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.21</v>
+        <v>3.08</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="P42" t="n">
-        <v>3.32</v>
+        <v>3.44</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -4300,15 +4300,15 @@
         </is>
       </c>
       <c r="R42" t="n">
-        <v>3.4</v>
+        <v>3.31</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>04/05/2023 02:42</t>
+          <t>04/05/2023 00:12</t>
         </is>
       </c>
       <c r="T42" t="n">
-        <v>4.16</v>
+        <v>4.11</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-avai/xlW7DvM5/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-esporte-clube-juventude/UNSaF0ig/</t>
         </is>
       </c>
     </row>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -4353,14 +4353,14 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I43" t="n">
         <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>2.21</v>
+        <v>1.89</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -4368,15 +4368,15 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>2.54</v>
+        <v>1.72</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>07/05/2023 01:23</t>
+          <t>07/05/2023 01:29</t>
         </is>
       </c>
       <c r="N43" t="n">
-        <v>3.13</v>
+        <v>3.24</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -4384,15 +4384,15 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>3.05</v>
+        <v>3.52</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>07/05/2023 01:23</t>
+          <t>07/05/2023 01:29</t>
         </is>
       </c>
       <c r="R43" t="n">
-        <v>3.47</v>
+        <v>4.42</v>
       </c>
       <c r="S43" t="inlineStr">
         <is>
@@ -4400,16 +4400,16 @@
         </is>
       </c>
       <c r="T43" t="n">
-        <v>3.21</v>
+        <v>5.77</v>
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>07/05/2023 01:23</t>
+          <t>07/05/2023 01:29</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-novorizontino/OpS3EK6a/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-abc/KCLCCbyC/</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -4445,14 +4445,14 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I44" t="n">
         <v>1</v>
       </c>
       <c r="J44" t="n">
-        <v>1.89</v>
+        <v>2.21</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -4460,15 +4460,15 @@
         </is>
       </c>
       <c r="L44" t="n">
-        <v>1.72</v>
+        <v>2.54</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>07/05/2023 01:29</t>
+          <t>07/05/2023 01:23</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>3.24</v>
+        <v>3.13</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -4476,15 +4476,15 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>3.52</v>
+        <v>3.05</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>07/05/2023 01:29</t>
+          <t>07/05/2023 01:23</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>4.42</v>
+        <v>3.47</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
@@ -4492,16 +4492,16 @@
         </is>
       </c>
       <c r="T44" t="n">
-        <v>5.77</v>
+        <v>3.21</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>07/05/2023 01:29</t>
+          <t>07/05/2023 01:23</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-abc/KCLCCbyC/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-novorizontino/OpS3EK6a/</t>
         </is>
       </c>
     </row>
@@ -6921,22 +6921,22 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I71" t="n">
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>2.19</v>
+        <v>1.69</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
@@ -6944,15 +6944,15 @@
         </is>
       </c>
       <c r="L71" t="n">
-        <v>2.5</v>
+        <v>1.71</v>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>24/05/2023 02:29</t>
+          <t>24/05/2023 02:21</t>
         </is>
       </c>
       <c r="N71" t="n">
-        <v>3.17</v>
+        <v>3.5</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -6960,15 +6960,15 @@
         </is>
       </c>
       <c r="P71" t="n">
-        <v>3.09</v>
+        <v>3.66</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>24/05/2023 02:23</t>
+          <t>24/05/2023 02:21</t>
         </is>
       </c>
       <c r="R71" t="n">
-        <v>3.46</v>
+        <v>5.26</v>
       </c>
       <c r="S71" t="inlineStr">
         <is>
@@ -6976,16 +6976,16 @@
         </is>
       </c>
       <c r="T71" t="n">
-        <v>3.23</v>
+        <v>5.62</v>
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>24/05/2023 02:29</t>
+          <t>24/05/2023 02:21</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-tombense/vXOXHEUl/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-avai/b1klwP0c/</t>
         </is>
       </c>
     </row>
@@ -7013,22 +7013,22 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="I72" t="n">
         <v>0</v>
       </c>
       <c r="J72" t="n">
-        <v>1.69</v>
+        <v>2.19</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -7036,15 +7036,15 @@
         </is>
       </c>
       <c r="L72" t="n">
-        <v>1.71</v>
+        <v>2.5</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>24/05/2023 02:21</t>
+          <t>24/05/2023 02:29</t>
         </is>
       </c>
       <c r="N72" t="n">
-        <v>3.5</v>
+        <v>3.17</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -7052,15 +7052,15 @@
         </is>
       </c>
       <c r="P72" t="n">
-        <v>3.66</v>
+        <v>3.09</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>24/05/2023 02:21</t>
+          <t>24/05/2023 02:23</t>
         </is>
       </c>
       <c r="R72" t="n">
-        <v>5.26</v>
+        <v>3.46</v>
       </c>
       <c r="S72" t="inlineStr">
         <is>
@@ -7068,16 +7068,16 @@
         </is>
       </c>
       <c r="T72" t="n">
-        <v>5.62</v>
+        <v>3.23</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>24/05/2023 02:21</t>
+          <t>24/05/2023 02:29</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-avai/b1klwP0c/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-tombense/vXOXHEUl/</t>
         </is>
       </c>
     </row>
@@ -7105,62 +7105,62 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="I73" t="n">
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>1.78</v>
+        <v>2.5</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>21/05/2023 23:42</t>
+          <t>21/05/2023 16:12</t>
         </is>
       </c>
       <c r="L73" t="n">
-        <v>1.71</v>
+        <v>2.15</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>24/05/2023 23:37</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="N73" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>21/05/2023 16:12</t>
+        </is>
+      </c>
+      <c r="P73" t="n">
         <v>3.35</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>21/05/2023 23:42</t>
-        </is>
-      </c>
-      <c r="P73" t="n">
-        <v>3.41</v>
-      </c>
       <c r="Q73" t="inlineStr">
         <is>
           <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="R73" t="n">
-        <v>4.92</v>
+        <v>3.1</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
-          <t>21/05/2023 23:42</t>
+          <t>21/05/2023 16:12</t>
         </is>
       </c>
       <c r="T73" t="n">
-        <v>5.69</v>
+        <v>3.7</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-crb/SzfhxqG3/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-atletico-go/ljr1zNpG/</t>
         </is>
       </c>
     </row>
@@ -7197,7 +7197,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -7205,14 +7205,14 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="I74" t="n">
         <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>1.84</v>
+        <v>1.78</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -7220,15 +7220,15 @@
         </is>
       </c>
       <c r="L74" t="n">
-        <v>1.77</v>
+        <v>1.71</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:56</t>
+          <t>24/05/2023 23:37</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.32</v>
+        <v>3.35</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -7236,15 +7236,15 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.39</v>
+        <v>3.41</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:53</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>4.98</v>
+        <v>4.92</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
@@ -7252,16 +7252,16 @@
         </is>
       </c>
       <c r="T74" t="n">
-        <v>5.65</v>
+        <v>5.69</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>24/05/2023 23:56</t>
+          <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ituano/428cG1gp/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-crb/SzfhxqG3/</t>
         </is>
       </c>
     </row>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -7297,63 +7297,63 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>2.67</v>
+        <v>1.84</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>2.83</v>
+        <v>1.77</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:56</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>2.98</v>
+        <v>3.32</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.12</v>
+        <v>3.39</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:53</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>3</v>
+        <v>4.98</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:42</t>
         </is>
       </c>
       <c r="T75" t="n">
-        <v>2.79</v>
+        <v>5.65</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>24/05/2023 23:58</t>
+          <t>24/05/2023 23:56</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-ceara/pAPTIfFr/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ituano/428cG1gp/</t>
         </is>
       </c>
     </row>
@@ -7381,30 +7381,30 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="G76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Ceara</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
         <v>3</v>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Atletico GO</t>
-        </is>
-      </c>
-      <c r="I76" t="n">
-        <v>0</v>
-      </c>
       <c r="J76" t="n">
-        <v>2.5</v>
+        <v>2.67</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>21/05/2023 16:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2.15</v>
+        <v>2.83</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
@@ -7412,40 +7412,40 @@
         </is>
       </c>
       <c r="N76" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>21/05/2023 20:42</t>
+        </is>
+      </c>
+      <c r="P76" t="n">
         <v>3.12</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>21/05/2023 16:12</t>
-        </is>
-      </c>
-      <c r="P76" t="n">
-        <v>3.35</v>
-      </c>
       <c r="Q76" t="inlineStr">
         <is>
           <t>24/05/2023 23:59</t>
         </is>
       </c>
       <c r="R76" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>21/05/2023 16:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="T76" t="n">
-        <v>3.7</v>
+        <v>2.79</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>24/05/2023 23:59</t>
+          <t>24/05/2023 23:58</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-atletico-go/ljr1zNpG/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-ceara/pAPTIfFr/</t>
         </is>
       </c>
     </row>
@@ -7565,71 +7565,71 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I78" t="n">
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>2.28</v>
+        <v>2.31</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="L78" t="n">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:28</t>
         </is>
       </c>
       <c r="N78" t="n">
-        <v>3.09</v>
+        <v>3.17</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="P78" t="n">
-        <v>3.08</v>
+        <v>3.03</v>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:29</t>
         </is>
       </c>
       <c r="R78" t="n">
-        <v>3.35</v>
+        <v>3.21</v>
       </c>
       <c r="S78" t="inlineStr">
         <is>
-          <t>21/05/2023 23:12</t>
+          <t>21/05/2023 20:42</t>
         </is>
       </c>
       <c r="T78" t="n">
-        <v>3.78</v>
+        <v>3.39</v>
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>25/05/2023 02:19</t>
+          <t>25/05/2023 02:28</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ponte-preta/6Rhdy3V9/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sport-recife/I5C1FL8j/</t>
         </is>
       </c>
     </row>
@@ -7657,71 +7657,71 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="I79" t="n">
         <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>2.31</v>
+        <v>2.28</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>2.45</v>
+        <v>2.25</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:28</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>3.17</v>
+        <v>3.09</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="P79" t="n">
-        <v>3.03</v>
+        <v>3.08</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:29</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>3.21</v>
+        <v>3.35</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>21/05/2023 20:42</t>
+          <t>21/05/2023 23:12</t>
         </is>
       </c>
       <c r="T79" t="n">
-        <v>3.39</v>
+        <v>3.78</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>25/05/2023 02:28</t>
+          <t>25/05/2023 02:19</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-sport-recife/I5C1FL8j/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ponte-preta/6Rhdy3V9/</t>
         </is>
       </c>
     </row>
@@ -7749,22 +7749,22 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G80" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Londrina</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
         <v>1</v>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Juventude</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>2</v>
-      </c>
       <c r="J80" t="n">
-        <v>2.12</v>
+        <v>2.08</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -7772,15 +7772,15 @@
         </is>
       </c>
       <c r="L80" t="n">
-        <v>2.53</v>
+        <v>1.97</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>27/05/2023 21:52</t>
+          <t>27/05/2023 21:31</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>3.22</v>
+        <v>3.14</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -7788,15 +7788,15 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>3.08</v>
+        <v>3.24</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>27/05/2023 21:52</t>
+          <t>27/05/2023 21:31</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>3.57</v>
+        <v>3.8</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
@@ -7804,16 +7804,16 @@
         </is>
       </c>
       <c r="T80" t="n">
-        <v>3.2</v>
+        <v>4.56</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>27/05/2023 21:52</t>
+          <t>27/05/2023 22:00</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-esporte-clube-juventude/f9YFUiEf/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-londrina/Sh5Swdi8/</t>
         </is>
       </c>
     </row>
@@ -7841,22 +7841,22 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J81" t="n">
-        <v>2.08</v>
+        <v>2.12</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -7864,15 +7864,15 @@
         </is>
       </c>
       <c r="L81" t="n">
-        <v>1.97</v>
+        <v>2.53</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>27/05/2023 21:31</t>
+          <t>27/05/2023 21:52</t>
         </is>
       </c>
       <c r="N81" t="n">
-        <v>3.14</v>
+        <v>3.22</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -7880,15 +7880,15 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>3.24</v>
+        <v>3.08</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>27/05/2023 21:31</t>
+          <t>27/05/2023 21:52</t>
         </is>
       </c>
       <c r="R81" t="n">
-        <v>3.8</v>
+        <v>3.57</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
@@ -7896,16 +7896,16 @@
         </is>
       </c>
       <c r="T81" t="n">
-        <v>4.56</v>
+        <v>3.2</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>27/05/2023 22:00</t>
+          <t>27/05/2023 21:52</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-londrina/Sh5Swdi8/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-esporte-clube-juventude/f9YFUiEf/</t>
         </is>
       </c>
     </row>
@@ -8209,22 +8209,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G85" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Criciuma</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
         <v>0</v>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Novorizontino</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>3</v>
-      </c>
       <c r="J85" t="n">
-        <v>2.05</v>
+        <v>2.04</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.09</v>
+        <v>2</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:20</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.22</v>
+        <v>3.36</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.18</v>
+        <v>3.31</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:29</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>3.8</v>
+        <v>4.05</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>4.15</v>
+        <v>4.3</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>28/05/2023 20:29</t>
+          <t>28/05/2023 20:21</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-novorizontino/2BcuyfyR/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-criciuma/td9WxG6E/</t>
         </is>
       </c>
     </row>
@@ -8301,22 +8301,22 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J86" t="n">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -8324,15 +8324,15 @@
         </is>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>2.09</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:20</t>
         </is>
       </c>
       <c r="N86" t="n">
-        <v>3.36</v>
+        <v>3.22</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -8340,15 +8340,15 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>3.31</v>
+        <v>3.18</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:29</t>
         </is>
       </c>
       <c r="R86" t="n">
-        <v>4.05</v>
+        <v>3.8</v>
       </c>
       <c r="S86" t="inlineStr">
         <is>
@@ -8356,16 +8356,16 @@
         </is>
       </c>
       <c r="T86" t="n">
-        <v>4.3</v>
+        <v>4.15</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>28/05/2023 20:21</t>
+          <t>28/05/2023 20:29</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-criciuma/td9WxG6E/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-novorizontino/2BcuyfyR/</t>
         </is>
       </c>
     </row>
@@ -8669,22 +8669,22 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="I90" t="n">
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>1.7</v>
+        <v>2.09</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>1.61</v>
+        <v>2.05</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:58</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.48</v>
+        <v>3.28</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.87</v>
+        <v>3.36</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:58</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>5.2</v>
+        <v>3.61</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>6.37</v>
+        <v>4.03</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>02/06/2023 23:34</t>
+          <t>02/06/2023 23:59</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-chapecoense-sc/Qm9ppXDs/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-tombense/IsKAjZzE/</t>
         </is>
       </c>
     </row>
@@ -8761,22 +8761,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="I91" t="n">
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>2.09</v>
+        <v>1.7</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>2.05</v>
+        <v>1.61</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:58</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>3.28</v>
+        <v>3.48</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>3.36</v>
+        <v>3.87</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:58</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>3.61</v>
+        <v>5.2</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>4.03</v>
+        <v>6.37</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>02/06/2023 23:59</t>
+          <t>02/06/2023 23:34</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-tombense/IsKAjZzE/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ceara-chapecoense-sc/Qm9ppXDs/</t>
         </is>
       </c>
     </row>
@@ -9129,22 +9129,22 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Novorizontino</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
         <v>1</v>
       </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Ponte Preta</t>
-        </is>
-      </c>
-      <c r="I95" t="n">
-        <v>0</v>
-      </c>
       <c r="J95" t="n">
-        <v>1.85</v>
+        <v>2.9</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,15 +9152,15 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>1.79</v>
+        <v>3.82</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>03/06/2023 21:55</t>
+          <t>03/06/2023 21:53</t>
         </is>
       </c>
       <c r="N95" t="n">
-        <v>3.3</v>
+        <v>3.13</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -9168,15 +9168,15 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>3.56</v>
+        <v>3.03</v>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>03/06/2023 21:55</t>
+          <t>03/06/2023 21:53</t>
         </is>
       </c>
       <c r="R95" t="n">
-        <v>4.55</v>
+        <v>2.53</v>
       </c>
       <c r="S95" t="inlineStr">
         <is>
@@ -9184,16 +9184,16 @@
         </is>
       </c>
       <c r="T95" t="n">
-        <v>5.11</v>
+        <v>2.26</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>03/06/2023 21:55</t>
+          <t>03/06/2023 21:53</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-ponte-preta/dYIEkgjK/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-novorizontino/Gx2csVc0/</t>
         </is>
       </c>
     </row>
@@ -9221,22 +9221,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G96" t="n">
+        <v>1</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Ponte Preta</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
         <v>0</v>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Novorizontino</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>1</v>
-      </c>
       <c r="J96" t="n">
-        <v>2.9</v>
+        <v>1.85</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>3.82</v>
+        <v>1.79</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>03/06/2023 21:53</t>
+          <t>03/06/2023 21:55</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.13</v>
+        <v>3.3</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,15 +9260,15 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.03</v>
+        <v>3.56</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>03/06/2023 21:53</t>
+          <t>03/06/2023 21:55</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.53</v>
+        <v>4.55</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.26</v>
+        <v>5.11</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>03/06/2023 21:53</t>
+          <t>03/06/2023 21:55</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-novorizontino/Gx2csVc0/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-ponte-preta/dYIEkgjK/</t>
         </is>
       </c>
     </row>
@@ -10693,7 +10693,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="G112" t="n">
@@ -10701,63 +10701,63 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="I112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>2.51</v>
+        <v>1.56</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>07/06/2023 02:42</t>
+          <t>08/06/2023 14:42</t>
         </is>
       </c>
       <c r="L112" t="n">
-        <v>2.28</v>
+        <v>1.61</v>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>10/06/2023 21:51</t>
+          <t>10/06/2023 21:22</t>
         </is>
       </c>
       <c r="N112" t="n">
-        <v>3.03</v>
+        <v>3.64</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
-          <t>07/06/2023 02:42</t>
+          <t>08/06/2023 14:42</t>
         </is>
       </c>
       <c r="P112" t="n">
-        <v>3.22</v>
+        <v>3.81</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>10/06/2023 21:59</t>
+          <t>10/06/2023 21:22</t>
         </is>
       </c>
       <c r="R112" t="n">
-        <v>3.02</v>
+        <v>6.5</v>
       </c>
       <c r="S112" t="inlineStr">
         <is>
-          <t>07/06/2023 02:42</t>
+          <t>08/06/2023 14:42</t>
         </is>
       </c>
       <c r="T112" t="n">
-        <v>3.5</v>
+        <v>6.55</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>10/06/2023 21:59</t>
+          <t>10/06/2023 21:22</t>
         </is>
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-atletico-go/jVYRFk4P/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-sampaio-correa/QNPgB9Ct/</t>
         </is>
       </c>
     </row>
@@ -10785,7 +10785,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G113" t="n">
@@ -10793,63 +10793,63 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>1.56</v>
+        <v>2.51</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>08/06/2023 14:42</t>
+          <t>07/06/2023 02:42</t>
         </is>
       </c>
       <c r="L113" t="n">
-        <v>1.61</v>
+        <v>2.28</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>10/06/2023 21:22</t>
+          <t>10/06/2023 21:51</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>3.64</v>
+        <v>3.03</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
-          <t>08/06/2023 14:42</t>
+          <t>07/06/2023 02:42</t>
         </is>
       </c>
       <c r="P113" t="n">
-        <v>3.81</v>
+        <v>3.22</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>10/06/2023 21:22</t>
+          <t>10/06/2023 21:59</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>6.5</v>
+        <v>3.02</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
-          <t>08/06/2023 14:42</t>
+          <t>07/06/2023 02:42</t>
         </is>
       </c>
       <c r="T113" t="n">
-        <v>6.55</v>
+        <v>3.5</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>10/06/2023 21:22</t>
+          <t>10/06/2023 21:59</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-sampaio-correa/QNPgB9Ct/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-atletico-go/jVYRFk4P/</t>
         </is>
       </c>
     </row>
@@ -15385,71 +15385,71 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G163" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="I163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J163" t="n">
-        <v>2.64</v>
+        <v>1.99</v>
       </c>
       <c r="K163" t="inlineStr">
         <is>
-          <t>09/07/2023 23:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="L163" t="n">
-        <v>2.68</v>
+        <v>1.95</v>
       </c>
       <c r="M163" t="inlineStr">
         <is>
-          <t>15/07/2023 02:27</t>
+          <t>15/07/2023 02:21</t>
         </is>
       </c>
       <c r="N163" t="n">
-        <v>3.01</v>
+        <v>3.21</v>
       </c>
       <c r="O163" t="inlineStr">
         <is>
-          <t>09/07/2023 23:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="P163" t="n">
-        <v>2.99</v>
+        <v>3.2</v>
       </c>
       <c r="Q163" t="inlineStr">
         <is>
-          <t>15/07/2023 02:27</t>
+          <t>15/07/2023 02:20</t>
         </is>
       </c>
       <c r="R163" t="n">
-        <v>2.87</v>
+        <v>4.35</v>
       </c>
       <c r="S163" t="inlineStr">
         <is>
-          <t>09/07/2023 23:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="T163" t="n">
-        <v>3.07</v>
+        <v>4.74</v>
       </c>
       <c r="U163" t="inlineStr">
         <is>
-          <t>15/07/2023 02:29</t>
+          <t>15/07/2023 02:21</t>
         </is>
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-sport-recife/KlNQMIY6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ituano/KnWlRXPh/</t>
         </is>
       </c>
     </row>
@@ -15477,71 +15477,71 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="G164" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
-        <v>1.99</v>
+        <v>2.64</v>
       </c>
       <c r="K164" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>09/07/2023 23:11</t>
         </is>
       </c>
       <c r="L164" t="n">
-        <v>1.95</v>
+        <v>2.68</v>
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>15/07/2023 02:21</t>
+          <t>15/07/2023 02:27</t>
         </is>
       </c>
       <c r="N164" t="n">
-        <v>3.21</v>
+        <v>3.01</v>
       </c>
       <c r="O164" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>09/07/2023 23:11</t>
         </is>
       </c>
       <c r="P164" t="n">
-        <v>3.2</v>
+        <v>2.99</v>
       </c>
       <c r="Q164" t="inlineStr">
         <is>
-          <t>15/07/2023 02:20</t>
+          <t>15/07/2023 02:27</t>
         </is>
       </c>
       <c r="R164" t="n">
-        <v>4.35</v>
+        <v>2.87</v>
       </c>
       <c r="S164" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>09/07/2023 23:11</t>
         </is>
       </c>
       <c r="T164" t="n">
-        <v>4.74</v>
+        <v>3.07</v>
       </c>
       <c r="U164" t="inlineStr">
         <is>
-          <t>15/07/2023 02:21</t>
+          <t>15/07/2023 02:29</t>
         </is>
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-ituano/KnWlRXPh/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-sport-recife/KlNQMIY6/</t>
         </is>
       </c>
     </row>
@@ -15661,71 +15661,71 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="G166" t="n">
+        <v>1</v>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Vila Nova FC</t>
+        </is>
+      </c>
+      <c r="I166" t="n">
         <v>0</v>
       </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>Tombense</t>
-        </is>
-      </c>
-      <c r="I166" t="n">
-        <v>1</v>
-      </c>
       <c r="J166" t="n">
-        <v>2.01</v>
+        <v>3.53</v>
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>11/07/2023 01:11</t>
         </is>
       </c>
       <c r="L166" t="n">
-        <v>2.2</v>
+        <v>4.33</v>
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>15/07/2023 21:57</t>
+          <t>15/07/2023 21:56</t>
         </is>
       </c>
       <c r="N166" t="n">
-        <v>3.2</v>
+        <v>3.06</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>11/07/2023 01:11</t>
         </is>
       </c>
       <c r="P166" t="n">
-        <v>3.14</v>
+        <v>3.17</v>
       </c>
       <c r="Q166" t="inlineStr">
         <is>
-          <t>15/07/2023 21:57</t>
+          <t>15/07/2023 21:56</t>
         </is>
       </c>
       <c r="R166" t="n">
-        <v>4.29</v>
+        <v>2.21</v>
       </c>
       <c r="S166" t="inlineStr">
         <is>
-          <t>08/07/2023 23:12</t>
+          <t>11/07/2023 01:11</t>
         </is>
       </c>
       <c r="T166" t="n">
-        <v>3.83</v>
+        <v>2.05</v>
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>15/07/2023 21:57</t>
+          <t>15/07/2023 21:56</t>
         </is>
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-tombense/xQXLNbJ0/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-vila-nova-fc/QqZdPBf5/</t>
         </is>
       </c>
     </row>
@@ -15753,71 +15753,71 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="G167" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Tombense</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
         <v>1</v>
       </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>Vila Nova FC</t>
-        </is>
-      </c>
-      <c r="I167" t="n">
-        <v>0</v>
-      </c>
       <c r="J167" t="n">
-        <v>3.53</v>
+        <v>2.01</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>11/07/2023 01:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="L167" t="n">
-        <v>4.33</v>
+        <v>2.2</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>15/07/2023 21:56</t>
+          <t>15/07/2023 21:57</t>
         </is>
       </c>
       <c r="N167" t="n">
-        <v>3.06</v>
+        <v>3.2</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
-          <t>11/07/2023 01:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="P167" t="n">
-        <v>3.17</v>
+        <v>3.14</v>
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>15/07/2023 21:56</t>
+          <t>15/07/2023 21:57</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>2.21</v>
+        <v>4.29</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>11/07/2023 01:11</t>
+          <t>08/07/2023 23:12</t>
         </is>
       </c>
       <c r="T167" t="n">
-        <v>2.05</v>
+        <v>3.83</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>15/07/2023 21:56</t>
+          <t>15/07/2023 21:57</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-vila-nova-fc/QqZdPBf5/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-tombense/xQXLNbJ0/</t>
         </is>
       </c>
     </row>
@@ -16581,30 +16581,30 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="G176" t="n">
+        <v>2</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Sampaio Correa</t>
+        </is>
+      </c>
+      <c r="I176" t="n">
         <v>0</v>
       </c>
-      <c r="H176" t="inlineStr">
-        <is>
-          <t>Guarani</t>
-        </is>
-      </c>
-      <c r="I176" t="n">
-        <v>1</v>
-      </c>
       <c r="J176" t="n">
-        <v>2.6</v>
+        <v>2.2</v>
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="L176" t="n">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="M176" t="inlineStr">
         <is>
@@ -16612,31 +16612,31 @@
         </is>
       </c>
       <c r="N176" t="n">
-        <v>2.85</v>
+        <v>3.05</v>
       </c>
       <c r="O176" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="P176" t="n">
-        <v>2.81</v>
+        <v>2.98</v>
       </c>
       <c r="Q176" t="inlineStr">
         <is>
-          <t>20/07/2023 02:26</t>
+          <t>20/07/2023 02:29</t>
         </is>
       </c>
       <c r="R176" t="n">
-        <v>3.08</v>
+        <v>3.82</v>
       </c>
       <c r="S176" t="inlineStr">
         <is>
-          <t>15/07/2023 16:12</t>
+          <t>15/07/2023 02:42</t>
         </is>
       </c>
       <c r="T176" t="n">
-        <v>3.42</v>
+        <v>4.71</v>
       </c>
       <c r="U176" t="inlineStr">
         <is>
@@ -16645,7 +16645,7 @@
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-guarani/KS9yy9gH/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-sampaio-correa/fPQDLTgU/</t>
         </is>
       </c>
     </row>
@@ -16673,30 +16673,30 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J177" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>15/07/2023 02:42</t>
+          <t>15/07/2023 16:12</t>
         </is>
       </c>
       <c r="L177" t="n">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="M177" t="inlineStr">
         <is>
@@ -16704,40 +16704,40 @@
         </is>
       </c>
       <c r="N177" t="n">
-        <v>3.05</v>
+        <v>2.85</v>
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>15/07/2023 02:42</t>
+          <t>15/07/2023 16:12</t>
         </is>
       </c>
       <c r="P177" t="n">
-        <v>2.98</v>
+        <v>2.81</v>
       </c>
       <c r="Q177" t="inlineStr">
         <is>
+          <t>20/07/2023 02:26</t>
+        </is>
+      </c>
+      <c r="R177" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S177" t="inlineStr">
+        <is>
+          <t>15/07/2023 16:12</t>
+        </is>
+      </c>
+      <c r="T177" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="U177" t="inlineStr">
+        <is>
           <t>20/07/2023 02:29</t>
         </is>
       </c>
-      <c r="R177" t="n">
-        <v>3.82</v>
-      </c>
-      <c r="S177" t="inlineStr">
-        <is>
-          <t>15/07/2023 02:42</t>
-        </is>
-      </c>
-      <c r="T177" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="U177" t="inlineStr">
-        <is>
-          <t>20/07/2023 02:29</t>
-        </is>
-      </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/avai-sampaio-correa/fPQDLTgU/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-guarani/KS9yy9gH/</t>
         </is>
       </c>
     </row>
@@ -17133,71 +17133,71 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I182" t="n">
         <v>1</v>
       </c>
       <c r="J182" t="n">
-        <v>1.49</v>
+        <v>2.7</v>
       </c>
       <c r="K182" t="inlineStr">
         <is>
-          <t>20/07/2023 02:42</t>
+          <t>20/07/2023 00:12</t>
         </is>
       </c>
       <c r="L182" t="n">
-        <v>1.47</v>
+        <v>2.57</v>
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>22/07/2023 21:49</t>
+          <t>22/07/2023 21:58</t>
         </is>
       </c>
       <c r="N182" t="n">
-        <v>4.17</v>
+        <v>2.87</v>
       </c>
       <c r="O182" t="inlineStr">
         <is>
-          <t>20/07/2023 02:42</t>
+          <t>20/07/2023 00:12</t>
         </is>
       </c>
       <c r="P182" t="n">
-        <v>3.98</v>
+        <v>2.92</v>
       </c>
       <c r="Q182" t="inlineStr">
         <is>
-          <t>22/07/2023 21:53</t>
+          <t>22/07/2023 21:58</t>
         </is>
       </c>
       <c r="R182" t="n">
-        <v>8</v>
+        <v>2.94</v>
       </c>
       <c r="S182" t="inlineStr">
         <is>
-          <t>20/07/2023 02:42</t>
+          <t>20/07/2023 00:12</t>
         </is>
       </c>
       <c r="T182" t="n">
-        <v>9.210000000000001</v>
+        <v>3.33</v>
       </c>
       <c r="U182" t="inlineStr">
         <is>
-          <t>22/07/2023 21:53</t>
+          <t>22/07/2023 21:58</t>
         </is>
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-abc/Gf3pZnOT/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-novorizontino/I3kCU6Wp/</t>
         </is>
       </c>
     </row>
@@ -17225,71 +17225,71 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I183" t="n">
         <v>1</v>
       </c>
       <c r="J183" t="n">
-        <v>2.7</v>
+        <v>1.49</v>
       </c>
       <c r="K183" t="inlineStr">
         <is>
-          <t>20/07/2023 00:12</t>
+          <t>20/07/2023 02:42</t>
         </is>
       </c>
       <c r="L183" t="n">
-        <v>2.57</v>
+        <v>1.47</v>
       </c>
       <c r="M183" t="inlineStr">
         <is>
-          <t>22/07/2023 21:58</t>
+          <t>22/07/2023 21:49</t>
         </is>
       </c>
       <c r="N183" t="n">
-        <v>2.87</v>
+        <v>4.17</v>
       </c>
       <c r="O183" t="inlineStr">
         <is>
-          <t>20/07/2023 00:12</t>
+          <t>20/07/2023 02:42</t>
         </is>
       </c>
       <c r="P183" t="n">
-        <v>2.92</v>
+        <v>3.98</v>
       </c>
       <c r="Q183" t="inlineStr">
         <is>
-          <t>22/07/2023 21:58</t>
+          <t>22/07/2023 21:53</t>
         </is>
       </c>
       <c r="R183" t="n">
-        <v>2.94</v>
+        <v>8</v>
       </c>
       <c r="S183" t="inlineStr">
         <is>
-          <t>20/07/2023 00:12</t>
+          <t>20/07/2023 02:42</t>
         </is>
       </c>
       <c r="T183" t="n">
-        <v>3.33</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="U183" t="inlineStr">
         <is>
-          <t>22/07/2023 21:58</t>
+          <t>22/07/2023 21:53</t>
         </is>
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-novorizontino/I3kCU6Wp/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-abc/Gf3pZnOT/</t>
         </is>
       </c>
     </row>
@@ -18789,46 +18789,46 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G200" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I200" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J200" t="n">
-        <v>1.57</v>
+        <v>2.02</v>
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="L200" t="n">
-        <v>1.66</v>
+        <v>2.09</v>
       </c>
       <c r="M200" t="inlineStr">
         <is>
-          <t>01/08/2023 23:33</t>
+          <t>01/08/2023 23:51</t>
         </is>
       </c>
       <c r="N200" t="n">
-        <v>3.79</v>
+        <v>3.06</v>
       </c>
       <c r="O200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="P200" t="n">
-        <v>3.68</v>
+        <v>3.06</v>
       </c>
       <c r="Q200" t="inlineStr">
         <is>
@@ -18836,24 +18836,24 @@
         </is>
       </c>
       <c r="R200" t="n">
-        <v>6.77</v>
+        <v>4.16</v>
       </c>
       <c r="S200" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>29/07/2023 23:12</t>
         </is>
       </c>
       <c r="T200" t="n">
-        <v>6.16</v>
+        <v>4.39</v>
       </c>
       <c r="U200" t="inlineStr">
         <is>
-          <t>01/08/2023 23:33</t>
+          <t>01/08/2023 23:51</t>
         </is>
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-avai/6cZMHQi3/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-botafogo-sp/SCNVF4MF/</t>
         </is>
       </c>
     </row>
@@ -18881,71 +18881,71 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J201" t="n">
-        <v>2.02</v>
+        <v>1.57</v>
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>29/07/2023 23:12</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="L201" t="n">
-        <v>2.09</v>
+        <v>1.66</v>
       </c>
       <c r="M201" t="inlineStr">
         <is>
+          <t>01/08/2023 23:33</t>
+        </is>
+      </c>
+      <c r="N201" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="O201" t="inlineStr">
+        <is>
+          <t>29/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P201" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
           <t>01/08/2023 23:51</t>
         </is>
       </c>
-      <c r="N201" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="O201" t="inlineStr">
-        <is>
-          <t>29/07/2023 23:12</t>
-        </is>
-      </c>
-      <c r="P201" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="Q201" t="inlineStr">
-        <is>
-          <t>01/08/2023 23:51</t>
-        </is>
-      </c>
       <c r="R201" t="n">
-        <v>4.16</v>
+        <v>6.77</v>
       </c>
       <c r="S201" t="inlineStr">
         <is>
-          <t>29/07/2023 23:12</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="T201" t="n">
-        <v>4.39</v>
+        <v>6.16</v>
       </c>
       <c r="U201" t="inlineStr">
         <is>
-          <t>01/08/2023 23:51</t>
+          <t>01/08/2023 23:33</t>
         </is>
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-botafogo-sp/SCNVF4MF/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-avai/6cZMHQi3/</t>
         </is>
       </c>
     </row>
@@ -19065,71 +19065,71 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G203" t="n">
+        <v>2</v>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>Ponte Preta</t>
+        </is>
+      </c>
+      <c r="I203" t="n">
         <v>1</v>
       </c>
-      <c r="H203" t="inlineStr">
-        <is>
-          <t>Tombense</t>
-        </is>
-      </c>
-      <c r="I203" t="n">
-        <v>0</v>
-      </c>
       <c r="J203" t="n">
-        <v>2.11</v>
+        <v>1.67</v>
       </c>
       <c r="K203" t="inlineStr">
         <is>
-          <t>30/07/2023 16:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="L203" t="n">
-        <v>2.14</v>
+        <v>1.73</v>
       </c>
       <c r="M203" t="inlineStr">
         <is>
-          <t>02/08/2023 23:58</t>
+          <t>02/08/2023 23:59</t>
         </is>
       </c>
       <c r="N203" t="n">
-        <v>3.17</v>
+        <v>3.34</v>
       </c>
       <c r="O203" t="inlineStr">
         <is>
-          <t>30/07/2023 16:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="P203" t="n">
-        <v>2.98</v>
+        <v>3.42</v>
       </c>
       <c r="Q203" t="inlineStr">
         <is>
-          <t>02/08/2023 23:58</t>
+          <t>02/08/2023 23:59</t>
         </is>
       </c>
       <c r="R203" t="n">
-        <v>3.68</v>
+        <v>5.96</v>
       </c>
       <c r="S203" t="inlineStr">
         <is>
-          <t>30/07/2023 16:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="T203" t="n">
-        <v>4.31</v>
+        <v>6.01</v>
       </c>
       <c r="U203" t="inlineStr">
         <is>
-          <t>02/08/2023 23:58</t>
+          <t>02/08/2023 23:59</t>
         </is>
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-tombense/fNVII6xc/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-ponte-preta/tKsyfNad/</t>
         </is>
       </c>
     </row>
@@ -19157,71 +19157,71 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G204" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="I204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J204" t="n">
-        <v>1.67</v>
+        <v>2.11</v>
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 16:12</t>
         </is>
       </c>
       <c r="L204" t="n">
-        <v>1.73</v>
+        <v>2.14</v>
       </c>
       <c r="M204" t="inlineStr">
         <is>
-          <t>02/08/2023 23:59</t>
+          <t>02/08/2023 23:58</t>
         </is>
       </c>
       <c r="N204" t="n">
-        <v>3.34</v>
+        <v>3.17</v>
       </c>
       <c r="O204" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 16:12</t>
         </is>
       </c>
       <c r="P204" t="n">
-        <v>3.42</v>
+        <v>2.98</v>
       </c>
       <c r="Q204" t="inlineStr">
         <is>
-          <t>02/08/2023 23:59</t>
+          <t>02/08/2023 23:58</t>
         </is>
       </c>
       <c r="R204" t="n">
-        <v>5.96</v>
+        <v>3.68</v>
       </c>
       <c r="S204" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 16:12</t>
         </is>
       </c>
       <c r="T204" t="n">
-        <v>6.01</v>
+        <v>4.31</v>
       </c>
       <c r="U204" t="inlineStr">
         <is>
-          <t>02/08/2023 23:59</t>
+          <t>02/08/2023 23:58</t>
         </is>
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-ponte-preta/tKsyfNad/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-tombense/fNVII6xc/</t>
         </is>
       </c>
     </row>
@@ -19249,7 +19249,7 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="G205" t="n">
@@ -19257,63 +19257,63 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Sport Recife</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J205" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="L205" t="n">
-        <v>2.31</v>
+        <v>2.1</v>
       </c>
       <c r="M205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:19</t>
+          <t>03/08/2023 02:28</t>
         </is>
       </c>
       <c r="N205" t="n">
-        <v>2.97</v>
+        <v>3.08</v>
       </c>
       <c r="O205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="P205" t="n">
-        <v>2.9</v>
+        <v>3.18</v>
       </c>
       <c r="Q205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:19</t>
+          <t>03/08/2023 02:24</t>
         </is>
       </c>
       <c r="R205" t="n">
-        <v>3.68</v>
+        <v>3.79</v>
       </c>
       <c r="S205" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="T205" t="n">
-        <v>3.9</v>
+        <v>4.11</v>
       </c>
       <c r="U205" t="inlineStr">
         <is>
-          <t>03/08/2023 02:27</t>
+          <t>03/08/2023 02:28</t>
         </is>
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-sport-recife/2TrXf3pj/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-ceara/phlSeqVq/</t>
         </is>
       </c>
     </row>
@@ -19341,7 +19341,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>Londrina</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="G206" t="n">
@@ -19349,26 +19349,26 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J206" t="n">
-        <v>2.51</v>
+        <v>2.38</v>
       </c>
       <c r="K206" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="L206" t="n">
-        <v>2.59</v>
+        <v>2.46</v>
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:21</t>
         </is>
       </c>
       <c r="N206" t="n">
@@ -19376,36 +19376,36 @@
       </c>
       <c r="O206" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="P206" t="n">
-        <v>2.9</v>
+        <v>2.94</v>
       </c>
       <c r="Q206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:28</t>
         </is>
       </c>
       <c r="R206" t="n">
-        <v>3.26</v>
+        <v>3.51</v>
       </c>
       <c r="S206" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="T206" t="n">
-        <v>3.31</v>
+        <v>3.48</v>
       </c>
       <c r="U206" t="inlineStr">
         <is>
-          <t>03/08/2023 02:18</t>
+          <t>03/08/2023 02:21</t>
         </is>
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-chapecoense-sc/YBk3cd6l/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-novorizontino/fLjabxir/</t>
         </is>
       </c>
     </row>
@@ -19433,71 +19433,71 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I207" t="n">
         <v>0</v>
       </c>
       <c r="J207" t="n">
-        <v>2.2</v>
+        <v>1.6</v>
       </c>
       <c r="K207" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="L207" t="n">
-        <v>2.1</v>
+        <v>1.47</v>
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>03/08/2023 02:28</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="N207" t="n">
-        <v>3.08</v>
+        <v>3.78</v>
       </c>
       <c r="O207" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="P207" t="n">
-        <v>3.18</v>
+        <v>4.23</v>
       </c>
       <c r="Q207" t="inlineStr">
         <is>
-          <t>03/08/2023 02:24</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="R207" t="n">
-        <v>3.79</v>
+        <v>5.67</v>
       </c>
       <c r="S207" t="inlineStr">
         <is>
-          <t>29/07/2023 22:12</t>
+          <t>30/07/2023 23:12</t>
         </is>
       </c>
       <c r="T207" t="n">
-        <v>4.11</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="U207" t="inlineStr">
         <is>
-          <t>03/08/2023 02:28</t>
+          <t>03/08/2023 02:29</t>
         </is>
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-ceara/phlSeqVq/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-abc/lMORGp79/</t>
         </is>
       </c>
     </row>
@@ -19525,7 +19525,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Londrina</t>
         </is>
       </c>
       <c r="G208" t="n">
@@ -19533,26 +19533,26 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="I208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J208" t="n">
-        <v>2.38</v>
+        <v>2.51</v>
       </c>
       <c r="K208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="L208" t="n">
-        <v>2.46</v>
+        <v>2.59</v>
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:21</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="N208" t="n">
@@ -19560,36 +19560,36 @@
       </c>
       <c r="O208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="P208" t="n">
-        <v>2.94</v>
+        <v>2.9</v>
       </c>
       <c r="Q208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:28</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="R208" t="n">
-        <v>3.51</v>
+        <v>3.26</v>
       </c>
       <c r="S208" t="inlineStr">
         <is>
-          <t>30/07/2023 20:42</t>
+          <t>29/07/2023 22:12</t>
         </is>
       </c>
       <c r="T208" t="n">
-        <v>3.48</v>
+        <v>3.31</v>
       </c>
       <c r="U208" t="inlineStr">
         <is>
-          <t>03/08/2023 02:21</t>
+          <t>03/08/2023 02:18</t>
         </is>
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-novorizontino/fLjabxir/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/londrina-chapecoense-sc/YBk3cd6l/</t>
         </is>
       </c>
     </row>
@@ -19617,71 +19617,71 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G209" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J209" t="n">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="L209" t="n">
-        <v>1.47</v>
+        <v>2.31</v>
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:19</t>
         </is>
       </c>
       <c r="N209" t="n">
-        <v>3.78</v>
+        <v>2.97</v>
       </c>
       <c r="O209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="P209" t="n">
-        <v>4.23</v>
+        <v>2.9</v>
       </c>
       <c r="Q209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:19</t>
         </is>
       </c>
       <c r="R209" t="n">
-        <v>5.67</v>
+        <v>3.68</v>
       </c>
       <c r="S209" t="inlineStr">
         <is>
-          <t>30/07/2023 23:12</t>
+          <t>30/07/2023 20:42</t>
         </is>
       </c>
       <c r="T209" t="n">
-        <v>8.199999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="U209" t="inlineStr">
         <is>
-          <t>03/08/2023 02:29</t>
+          <t>03/08/2023 02:27</t>
         </is>
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-abc/lMORGp79/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-sport-recife/2TrXf3pj/</t>
         </is>
       </c>
     </row>
@@ -22009,22 +22009,22 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="G235" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="I235" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J235" t="n">
-        <v>2.69</v>
+        <v>2.62</v>
       </c>
       <c r="K235" t="inlineStr">
         <is>
@@ -22032,7 +22032,7 @@
         </is>
       </c>
       <c r="L235" t="n">
-        <v>2.79</v>
+        <v>2.94</v>
       </c>
       <c r="M235" t="inlineStr">
         <is>
@@ -22040,7 +22040,7 @@
         </is>
       </c>
       <c r="N235" t="n">
-        <v>3</v>
+        <v>2.95</v>
       </c>
       <c r="O235" t="inlineStr">
         <is>
@@ -22048,32 +22048,32 @@
         </is>
       </c>
       <c r="P235" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>19/08/2023 21:57</t>
+        </is>
+      </c>
+      <c r="R235" t="n">
         <v>2.95</v>
       </c>
-      <c r="Q235" t="inlineStr">
+      <c r="S235" t="inlineStr">
+        <is>
+          <t>15/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T235" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="U235" t="inlineStr">
         <is>
           <t>19/08/2023 21:51</t>
         </is>
       </c>
-      <c r="R235" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="S235" t="inlineStr">
-        <is>
-          <t>15/08/2023 00:12</t>
-        </is>
-      </c>
-      <c r="T235" t="n">
-        <v>2.98</v>
-      </c>
-      <c r="U235" t="inlineStr">
-        <is>
-          <t>19/08/2023 21:51</t>
-        </is>
-      </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-criciuma/jmzKsEBP/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-crb/jBI6Y9YB/</t>
         </is>
       </c>
     </row>
@@ -22101,22 +22101,22 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="G236" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="I236" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>2.62</v>
+        <v>2.69</v>
       </c>
       <c r="K236" t="inlineStr">
         <is>
@@ -22124,7 +22124,7 @@
         </is>
       </c>
       <c r="L236" t="n">
-        <v>2.94</v>
+        <v>2.79</v>
       </c>
       <c r="M236" t="inlineStr">
         <is>
@@ -22132,31 +22132,31 @@
         </is>
       </c>
       <c r="N236" t="n">
+        <v>3</v>
+      </c>
+      <c r="O236" t="inlineStr">
+        <is>
+          <t>15/08/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P236" t="n">
         <v>2.95</v>
       </c>
-      <c r="O236" t="inlineStr">
+      <c r="Q236" t="inlineStr">
+        <is>
+          <t>19/08/2023 21:51</t>
+        </is>
+      </c>
+      <c r="R236" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="S236" t="inlineStr">
         <is>
           <t>15/08/2023 00:12</t>
         </is>
       </c>
-      <c r="P236" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="Q236" t="inlineStr">
-        <is>
-          <t>19/08/2023 21:57</t>
-        </is>
-      </c>
-      <c r="R236" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="S236" t="inlineStr">
-        <is>
-          <t>15/08/2023 00:12</t>
-        </is>
-      </c>
       <c r="T236" t="n">
-        <v>2.99</v>
+        <v>2.98</v>
       </c>
       <c r="U236" t="inlineStr">
         <is>
@@ -22165,7 +22165,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-crb/jBI6Y9YB/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ituano-criciuma/jmzKsEBP/</t>
         </is>
       </c>
     </row>
@@ -30013,71 +30013,71 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="I322" t="n">
         <v>1</v>
       </c>
       <c r="J322" t="n">
-        <v>1.35</v>
+        <v>2.81</v>
       </c>
       <c r="K322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="L322" t="n">
-        <v>1.39</v>
+        <v>3.42</v>
       </c>
       <c r="M322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:51</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="N322" t="n">
-        <v>4.58</v>
+        <v>2.86</v>
       </c>
       <c r="O322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="P322" t="n">
-        <v>4.61</v>
+        <v>2.91</v>
       </c>
       <c r="Q322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:58</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="R322" t="n">
-        <v>9.109999999999999</v>
+        <v>2.97</v>
       </c>
       <c r="S322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="T322" t="n">
-        <v>9.75</v>
+        <v>2.52</v>
       </c>
       <c r="U322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:58</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="V322" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-abc/YuRGMRij/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vila-nova-fc/8I9Nu7bS/</t>
         </is>
       </c>
     </row>
@@ -30105,71 +30105,71 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H323" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I323" t="n">
         <v>1</v>
       </c>
       <c r="J323" t="n">
-        <v>2.81</v>
+        <v>1.35</v>
       </c>
       <c r="K323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="L323" t="n">
-        <v>3.42</v>
+        <v>1.39</v>
       </c>
       <c r="M323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:51</t>
         </is>
       </c>
       <c r="N323" t="n">
-        <v>2.86</v>
+        <v>4.58</v>
       </c>
       <c r="O323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="P323" t="n">
-        <v>2.91</v>
+        <v>4.61</v>
       </c>
       <c r="Q323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:58</t>
         </is>
       </c>
       <c r="R323" t="n">
-        <v>2.97</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="S323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="T323" t="n">
-        <v>2.52</v>
+        <v>9.75</v>
       </c>
       <c r="U323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:58</t>
         </is>
       </c>
       <c r="V323" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vila-nova-fc/8I9Nu7bS/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-abc/YuRGMRij/</t>
         </is>
       </c>
     </row>
@@ -32221,71 +32221,71 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G346" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H346" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I346" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J346" t="n">
-        <v>2.33</v>
+        <v>2.41</v>
       </c>
       <c r="K346" t="inlineStr">
         <is>
-          <t>29/10/2023 02:42</t>
+          <t>29/10/2023 04:42</t>
         </is>
       </c>
       <c r="L346" t="n">
-        <v>2.52</v>
+        <v>2.28</v>
       </c>
       <c r="M346" t="inlineStr">
         <is>
-          <t>04/11/2023 20:45</t>
+          <t>04/11/2023 20:59</t>
         </is>
       </c>
       <c r="N346" t="n">
-        <v>2.97</v>
+        <v>2.88</v>
       </c>
       <c r="O346" t="inlineStr">
         <is>
-          <t>29/10/2023 02:42</t>
+          <t>29/10/2023 04:42</t>
         </is>
       </c>
       <c r="P346" t="n">
-        <v>2.86</v>
+        <v>2.98</v>
       </c>
       <c r="Q346" t="inlineStr">
         <is>
-          <t>04/11/2023 20:38</t>
+          <t>04/11/2023 20:59</t>
         </is>
       </c>
       <c r="R346" t="n">
-        <v>3.61</v>
+        <v>3.55</v>
       </c>
       <c r="S346" t="inlineStr">
         <is>
-          <t>29/10/2023 02:42</t>
+          <t>29/10/2023 04:42</t>
         </is>
       </c>
       <c r="T346" t="n">
-        <v>3.48</v>
+        <v>3.86</v>
       </c>
       <c r="U346" t="inlineStr">
         <is>
-          <t>04/11/2023 20:45</t>
+          <t>04/11/2023 20:59</t>
         </is>
       </c>
       <c r="V346" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-avai/SQpwzxS6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-ceara/xdSTdaZJ/</t>
         </is>
       </c>
     </row>
@@ -32313,71 +32313,71 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="G347" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H347" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I347" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J347" t="n">
-        <v>2.41</v>
+        <v>2.33</v>
       </c>
       <c r="K347" t="inlineStr">
         <is>
-          <t>29/10/2023 04:42</t>
+          <t>29/10/2023 02:42</t>
         </is>
       </c>
       <c r="L347" t="n">
-        <v>2.28</v>
+        <v>2.52</v>
       </c>
       <c r="M347" t="inlineStr">
         <is>
-          <t>04/11/2023 20:59</t>
+          <t>04/11/2023 20:45</t>
         </is>
       </c>
       <c r="N347" t="n">
-        <v>2.88</v>
+        <v>2.97</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
-          <t>29/10/2023 04:42</t>
+          <t>29/10/2023 02:42</t>
         </is>
       </c>
       <c r="P347" t="n">
-        <v>2.98</v>
+        <v>2.86</v>
       </c>
       <c r="Q347" t="inlineStr">
         <is>
-          <t>04/11/2023 20:59</t>
+          <t>04/11/2023 20:38</t>
         </is>
       </c>
       <c r="R347" t="n">
-        <v>3.55</v>
+        <v>3.61</v>
       </c>
       <c r="S347" t="inlineStr">
         <is>
-          <t>29/10/2023 04:42</t>
+          <t>29/10/2023 02:42</t>
         </is>
       </c>
       <c r="T347" t="n">
-        <v>3.86</v>
+        <v>3.48</v>
       </c>
       <c r="U347" t="inlineStr">
         <is>
-          <t>04/11/2023 20:59</t>
+          <t>04/11/2023 20:45</t>
         </is>
       </c>
       <c r="V347" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-ceara/xdSTdaZJ/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/ponte-preta-avai/SQpwzxS6/</t>
         </is>
       </c>
     </row>
@@ -33482,6 +33482,190 @@
       <c r="V359" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-vitoria/xEZzk5ht/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>serie-b</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E360" s="2" t="n">
+        <v>45244.95833333334</v>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>Guarani</t>
+        </is>
+      </c>
+      <c r="G360" t="n">
+        <v>1</v>
+      </c>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>Criciuma</t>
+        </is>
+      </c>
+      <c r="I360" t="n">
+        <v>1</v>
+      </c>
+      <c r="J360" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K360" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L360" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="M360" t="inlineStr">
+        <is>
+          <t>14/11/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N360" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="O360" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P360" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="Q360" t="inlineStr">
+        <is>
+          <t>14/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="R360" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="S360" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T360" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="U360" t="inlineStr">
+        <is>
+          <t>14/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="V360" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-criciuma/lfEKnFBC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>serie-b</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E361" s="2" t="n">
+        <v>45245.0625</v>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="G361" t="n">
+        <v>0</v>
+      </c>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>Juventude</t>
+        </is>
+      </c>
+      <c r="I361" t="n">
+        <v>0</v>
+      </c>
+      <c r="J361" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="K361" t="inlineStr">
+        <is>
+          <t>08/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="L361" t="n">
+        <v>7.03</v>
+      </c>
+      <c r="M361" t="inlineStr">
+        <is>
+          <t>15/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="N361" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="O361" t="inlineStr">
+        <is>
+          <t>08/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="P361" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="Q361" t="inlineStr">
+        <is>
+          <t>15/11/2023 01:27</t>
+        </is>
+      </c>
+      <c r="R361" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="S361" t="inlineStr">
+        <is>
+          <t>08/11/2023 05:42</t>
+        </is>
+      </c>
+      <c r="T361" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U361" t="inlineStr">
+        <is>
+          <t>15/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="V361" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/abc-esporte-clube-juventude/Ojmlps7B/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 21-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/brazil_serie-b_2023.xlsx
+++ b/2023/brazil_serie-b_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V370"/>
+  <dimension ref="A1:V371"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25781,71 +25781,71 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="I276" t="n">
         <v>0</v>
       </c>
       <c r="J276" t="n">
-        <v>2.08</v>
+        <v>2.92</v>
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>11/09/2023 02:42</t>
+          <t>11/09/2023 08:12</t>
         </is>
       </c>
       <c r="L276" t="n">
-        <v>2.12</v>
+        <v>3.52</v>
       </c>
       <c r="M276" t="inlineStr">
         <is>
+          <t>16/09/2023 21:52</t>
+        </is>
+      </c>
+      <c r="N276" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="O276" t="inlineStr">
+        <is>
+          <t>11/09/2023 08:12</t>
+        </is>
+      </c>
+      <c r="P276" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="Q276" t="inlineStr">
+        <is>
           <t>16/09/2023 21:50</t>
         </is>
       </c>
-      <c r="N276" t="n">
-        <v>2.96</v>
-      </c>
-      <c r="O276" t="inlineStr">
-        <is>
-          <t>11/09/2023 02:42</t>
-        </is>
-      </c>
-      <c r="P276" t="n">
-        <v>2.89</v>
-      </c>
-      <c r="Q276" t="inlineStr">
+      <c r="R276" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="S276" t="inlineStr">
+        <is>
+          <t>11/09/2023 08:12</t>
+        </is>
+      </c>
+      <c r="T276" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="U276" t="inlineStr">
         <is>
           <t>16/09/2023 21:50</t>
         </is>
       </c>
-      <c r="R276" t="n">
-        <v>4.43</v>
-      </c>
-      <c r="S276" t="inlineStr">
-        <is>
-          <t>11/09/2023 02:42</t>
-        </is>
-      </c>
-      <c r="T276" t="n">
-        <v>4.62</v>
-      </c>
-      <c r="U276" t="inlineStr">
-        <is>
-          <t>16/09/2023 21:50</t>
-        </is>
-      </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-chapecoense-sc/6gaZd5YQ/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-atletico-go/M5cNa7l8/</t>
         </is>
       </c>
     </row>
@@ -25873,46 +25873,46 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G277" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="I277" t="n">
         <v>0</v>
       </c>
       <c r="J277" t="n">
-        <v>2.92</v>
+        <v>2.08</v>
       </c>
       <c r="K277" t="inlineStr">
         <is>
-          <t>11/09/2023 08:12</t>
+          <t>11/09/2023 02:42</t>
         </is>
       </c>
       <c r="L277" t="n">
-        <v>3.52</v>
+        <v>2.12</v>
       </c>
       <c r="M277" t="inlineStr">
         <is>
-          <t>16/09/2023 21:52</t>
+          <t>16/09/2023 21:50</t>
         </is>
       </c>
       <c r="N277" t="n">
-        <v>2.79</v>
+        <v>2.96</v>
       </c>
       <c r="O277" t="inlineStr">
         <is>
-          <t>11/09/2023 08:12</t>
+          <t>11/09/2023 02:42</t>
         </is>
       </c>
       <c r="P277" t="n">
-        <v>2.88</v>
+        <v>2.89</v>
       </c>
       <c r="Q277" t="inlineStr">
         <is>
@@ -25920,15 +25920,15 @@
         </is>
       </c>
       <c r="R277" t="n">
-        <v>2.92</v>
+        <v>4.43</v>
       </c>
       <c r="S277" t="inlineStr">
         <is>
-          <t>11/09/2023 08:12</t>
+          <t>11/09/2023 02:42</t>
         </is>
       </c>
       <c r="T277" t="n">
-        <v>2.48</v>
+        <v>4.62</v>
       </c>
       <c r="U277" t="inlineStr">
         <is>
@@ -25937,7 +25937,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-atletico-go/M5cNa7l8/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-chapecoense-sc/6gaZd5YQ/</t>
         </is>
       </c>
     </row>
@@ -26701,7 +26701,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Chapecoense-SC</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G286" t="n">
@@ -26709,63 +26709,63 @@
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="I286" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J286" t="n">
-        <v>2.55</v>
+        <v>2.09</v>
       </c>
       <c r="K286" t="inlineStr">
         <is>
-          <t>19/09/2023 01:12</t>
+          <t>18/09/2023 20:13</t>
         </is>
       </c>
       <c r="L286" t="n">
-        <v>2.4</v>
+        <v>2.14</v>
       </c>
       <c r="M286" t="inlineStr">
         <is>
-          <t>23/09/2023 21:58</t>
+          <t>23/09/2023 21:53</t>
         </is>
       </c>
       <c r="N286" t="n">
-        <v>2.89</v>
+        <v>3.03</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
-          <t>19/09/2023 01:12</t>
+          <t>18/09/2023 20:13</t>
         </is>
       </c>
       <c r="P286" t="n">
-        <v>2.91</v>
+        <v>3.06</v>
       </c>
       <c r="Q286" t="inlineStr">
         <is>
-          <t>23/09/2023 21:59</t>
+          <t>23/09/2023 21:53</t>
         </is>
       </c>
       <c r="R286" t="n">
-        <v>3.27</v>
+        <v>4.27</v>
       </c>
       <c r="S286" t="inlineStr">
         <is>
-          <t>19/09/2023 01:12</t>
+          <t>18/09/2023 20:13</t>
         </is>
       </c>
       <c r="T286" t="n">
-        <v>3.67</v>
+        <v>4.15</v>
       </c>
       <c r="U286" t="inlineStr">
         <is>
-          <t>23/09/2023 21:59</t>
+          <t>23/09/2023 21:53</t>
         </is>
       </c>
       <c r="V286" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ceara/OfNy52Qm/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-guarani/KMGp3te0/</t>
         </is>
       </c>
     </row>
@@ -26793,7 +26793,7 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Chapecoense-SC</t>
         </is>
       </c>
       <c r="G287" t="n">
@@ -26801,63 +26801,63 @@
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J287" t="n">
-        <v>2.09</v>
+        <v>2.55</v>
       </c>
       <c r="K287" t="inlineStr">
         <is>
-          <t>18/09/2023 20:13</t>
+          <t>19/09/2023 01:12</t>
         </is>
       </c>
       <c r="L287" t="n">
-        <v>2.14</v>
+        <v>2.4</v>
       </c>
       <c r="M287" t="inlineStr">
         <is>
-          <t>23/09/2023 21:53</t>
+          <t>23/09/2023 21:58</t>
         </is>
       </c>
       <c r="N287" t="n">
-        <v>3.03</v>
+        <v>2.89</v>
       </c>
       <c r="O287" t="inlineStr">
         <is>
-          <t>18/09/2023 20:13</t>
+          <t>19/09/2023 01:12</t>
         </is>
       </c>
       <c r="P287" t="n">
-        <v>3.06</v>
+        <v>2.91</v>
       </c>
       <c r="Q287" t="inlineStr">
         <is>
-          <t>23/09/2023 21:53</t>
+          <t>23/09/2023 21:59</t>
         </is>
       </c>
       <c r="R287" t="n">
-        <v>4.27</v>
+        <v>3.27</v>
       </c>
       <c r="S287" t="inlineStr">
         <is>
-          <t>18/09/2023 20:13</t>
+          <t>19/09/2023 01:12</t>
         </is>
       </c>
       <c r="T287" t="n">
-        <v>4.15</v>
+        <v>3.67</v>
       </c>
       <c r="U287" t="inlineStr">
         <is>
-          <t>23/09/2023 21:53</t>
+          <t>23/09/2023 21:59</t>
         </is>
       </c>
       <c r="V287" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-guarani/KMGp3te0/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/chapecoense-sc-ceara/OfNy52Qm/</t>
         </is>
       </c>
     </row>
@@ -28357,22 +28357,22 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>CRB</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H304" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Ituano</t>
         </is>
       </c>
       <c r="I304" t="n">
         <v>0</v>
       </c>
       <c r="J304" t="n">
-        <v>2.2</v>
+        <v>1.66</v>
       </c>
       <c r="K304" t="inlineStr">
         <is>
@@ -28380,15 +28380,15 @@
         </is>
       </c>
       <c r="L304" t="n">
-        <v>2.01</v>
+        <v>1.63</v>
       </c>
       <c r="M304" t="inlineStr">
         <is>
-          <t>07/10/2023 02:24</t>
+          <t>07/10/2023 02:26</t>
         </is>
       </c>
       <c r="N304" t="n">
-        <v>3.02</v>
+        <v>3.63</v>
       </c>
       <c r="O304" t="inlineStr">
         <is>
@@ -28396,15 +28396,15 @@
         </is>
       </c>
       <c r="P304" t="n">
-        <v>3.26</v>
+        <v>3.77</v>
       </c>
       <c r="Q304" t="inlineStr">
         <is>
-          <t>07/10/2023 02:24</t>
+          <t>07/10/2023 02:26</t>
         </is>
       </c>
       <c r="R304" t="n">
-        <v>3.87</v>
+        <v>5.97</v>
       </c>
       <c r="S304" t="inlineStr">
         <is>
@@ -28412,16 +28412,16 @@
         </is>
       </c>
       <c r="T304" t="n">
-        <v>4.36</v>
+        <v>6.24</v>
       </c>
       <c r="U304" t="inlineStr">
         <is>
-          <t>07/10/2023 02:24</t>
+          <t>07/10/2023 02:26</t>
         </is>
       </c>
       <c r="V304" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-ceara/IgpBFApN/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-ituano/OWOy1BVT/</t>
         </is>
       </c>
     </row>
@@ -28449,22 +28449,22 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>CRB</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H305" t="inlineStr">
         <is>
-          <t>Ituano</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I305" t="n">
         <v>0</v>
       </c>
       <c r="J305" t="n">
-        <v>1.66</v>
+        <v>2.2</v>
       </c>
       <c r="K305" t="inlineStr">
         <is>
@@ -28472,15 +28472,15 @@
         </is>
       </c>
       <c r="L305" t="n">
-        <v>1.63</v>
+        <v>2.01</v>
       </c>
       <c r="M305" t="inlineStr">
         <is>
-          <t>07/10/2023 02:26</t>
+          <t>07/10/2023 02:24</t>
         </is>
       </c>
       <c r="N305" t="n">
-        <v>3.63</v>
+        <v>3.02</v>
       </c>
       <c r="O305" t="inlineStr">
         <is>
@@ -28488,15 +28488,15 @@
         </is>
       </c>
       <c r="P305" t="n">
-        <v>3.77</v>
+        <v>3.26</v>
       </c>
       <c r="Q305" t="inlineStr">
         <is>
-          <t>07/10/2023 02:26</t>
+          <t>07/10/2023 02:24</t>
         </is>
       </c>
       <c r="R305" t="n">
-        <v>5.97</v>
+        <v>3.87</v>
       </c>
       <c r="S305" t="inlineStr">
         <is>
@@ -28504,16 +28504,16 @@
         </is>
       </c>
       <c r="T305" t="n">
-        <v>6.24</v>
+        <v>4.36</v>
       </c>
       <c r="U305" t="inlineStr">
         <is>
-          <t>07/10/2023 02:26</t>
+          <t>07/10/2023 02:24</t>
         </is>
       </c>
       <c r="V305" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-ituano/OWOy1BVT/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/crb-ceara/IgpBFApN/</t>
         </is>
       </c>
     </row>
@@ -28633,22 +28633,22 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Sampaio Correa</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="G307" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Avai</t>
         </is>
       </c>
       <c r="I307" t="n">
         <v>1</v>
       </c>
       <c r="J307" t="n">
-        <v>3.32</v>
+        <v>2.02</v>
       </c>
       <c r="K307" t="inlineStr">
         <is>
@@ -28656,15 +28656,15 @@
         </is>
       </c>
       <c r="L307" t="n">
-        <v>3.03</v>
+        <v>2.05</v>
       </c>
       <c r="M307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:59</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="N307" t="n">
-        <v>2.94</v>
+        <v>3.01</v>
       </c>
       <c r="O307" t="inlineStr">
         <is>
@@ -28672,15 +28672,15 @@
         </is>
       </c>
       <c r="P307" t="n">
-        <v>2.89</v>
+        <v>3.04</v>
       </c>
       <c r="Q307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:51</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="R307" t="n">
-        <v>2.39</v>
+        <v>4.62</v>
       </c>
       <c r="S307" t="inlineStr">
         <is>
@@ -28688,16 +28688,16 @@
         </is>
       </c>
       <c r="T307" t="n">
-        <v>2.8</v>
+        <v>4.58</v>
       </c>
       <c r="U307" t="inlineStr">
         <is>
-          <t>07/10/2023 21:59</t>
+          <t>07/10/2023 21:58</t>
         </is>
       </c>
       <c r="V307" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-novorizontino/S4ibIC04/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-avai/hnaoLEGo/</t>
         </is>
       </c>
     </row>
@@ -28725,22 +28725,22 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sampaio Correa</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>Avai</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="I308" t="n">
         <v>1</v>
       </c>
       <c r="J308" t="n">
-        <v>2.02</v>
+        <v>3.32</v>
       </c>
       <c r="K308" t="inlineStr">
         <is>
@@ -28748,15 +28748,15 @@
         </is>
       </c>
       <c r="L308" t="n">
-        <v>2.05</v>
+        <v>3.03</v>
       </c>
       <c r="M308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:59</t>
         </is>
       </c>
       <c r="N308" t="n">
-        <v>3.01</v>
+        <v>2.94</v>
       </c>
       <c r="O308" t="inlineStr">
         <is>
@@ -28764,15 +28764,15 @@
         </is>
       </c>
       <c r="P308" t="n">
-        <v>3.04</v>
+        <v>2.89</v>
       </c>
       <c r="Q308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:51</t>
         </is>
       </c>
       <c r="R308" t="n">
-        <v>4.62</v>
+        <v>2.39</v>
       </c>
       <c r="S308" t="inlineStr">
         <is>
@@ -28780,16 +28780,16 @@
         </is>
       </c>
       <c r="T308" t="n">
-        <v>4.58</v>
+        <v>2.8</v>
       </c>
       <c r="U308" t="inlineStr">
         <is>
-          <t>07/10/2023 21:58</t>
+          <t>07/10/2023 21:59</t>
         </is>
       </c>
       <c r="V308" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/botafogo-sp-avai/hnaoLEGo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-novorizontino/S4ibIC04/</t>
         </is>
       </c>
     </row>
@@ -30013,71 +30013,71 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Tombense</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="I322" t="n">
         <v>1</v>
       </c>
       <c r="J322" t="n">
-        <v>1.35</v>
+        <v>2.81</v>
       </c>
       <c r="K322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="L322" t="n">
-        <v>1.39</v>
+        <v>3.42</v>
       </c>
       <c r="M322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:51</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="N322" t="n">
-        <v>4.58</v>
+        <v>2.86</v>
       </c>
       <c r="O322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="P322" t="n">
-        <v>4.61</v>
+        <v>2.91</v>
       </c>
       <c r="Q322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:58</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="R322" t="n">
-        <v>9.109999999999999</v>
+        <v>2.97</v>
       </c>
       <c r="S322" t="inlineStr">
         <is>
-          <t>15/10/2023 20:12</t>
+          <t>14/10/2023 21:13</t>
         </is>
       </c>
       <c r="T322" t="n">
-        <v>9.75</v>
+        <v>2.52</v>
       </c>
       <c r="U322" t="inlineStr">
         <is>
-          <t>19/10/2023 23:58</t>
+          <t>19/10/2023 23:47</t>
         </is>
       </c>
       <c r="V322" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-abc/YuRGMRij/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vila-nova-fc/8I9Nu7bS/</t>
         </is>
       </c>
     </row>
@@ -30105,71 +30105,71 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Tombense</t>
+          <t>Atletico GO</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H323" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="I323" t="n">
         <v>1</v>
       </c>
       <c r="J323" t="n">
-        <v>2.81</v>
+        <v>1.35</v>
       </c>
       <c r="K323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="L323" t="n">
-        <v>3.42</v>
+        <v>1.39</v>
       </c>
       <c r="M323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:51</t>
         </is>
       </c>
       <c r="N323" t="n">
-        <v>2.86</v>
+        <v>4.58</v>
       </c>
       <c r="O323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="P323" t="n">
-        <v>2.91</v>
+        <v>4.61</v>
       </c>
       <c r="Q323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:58</t>
         </is>
       </c>
       <c r="R323" t="n">
-        <v>2.97</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="S323" t="inlineStr">
         <is>
-          <t>14/10/2023 21:13</t>
+          <t>15/10/2023 20:12</t>
         </is>
       </c>
       <c r="T323" t="n">
-        <v>2.52</v>
+        <v>9.75</v>
       </c>
       <c r="U323" t="inlineStr">
         <is>
-          <t>19/10/2023 23:47</t>
+          <t>19/10/2023 23:58</t>
         </is>
       </c>
       <c r="V323" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/tombense-vila-nova-fc/8I9Nu7bS/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/atletico-go-abc/YuRGMRij/</t>
         </is>
       </c>
     </row>
@@ -31117,71 +31117,71 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Novorizontino</t>
+          <t>Guarani</t>
         </is>
       </c>
       <c r="G334" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J334" t="n">
-        <v>1.53</v>
+        <v>1.64</v>
       </c>
       <c r="K334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="L334" t="n">
-        <v>1.39</v>
+        <v>1.7</v>
       </c>
       <c r="M334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:21</t>
+          <t>28/10/2023 02:05</t>
         </is>
       </c>
       <c r="N334" t="n">
-        <v>3.81</v>
+        <v>3.41</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="P334" t="n">
-        <v>4.57</v>
+        <v>3.43</v>
       </c>
       <c r="Q334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:28</t>
+          <t>28/10/2023 02:17</t>
         </is>
       </c>
       <c r="R334" t="n">
-        <v>6.57</v>
+        <v>6.14</v>
       </c>
       <c r="S334" t="inlineStr">
         <is>
-          <t>24/10/2023 01:12</t>
+          <t>21/10/2023 22:12</t>
         </is>
       </c>
       <c r="T334" t="n">
-        <v>10.13</v>
+        <v>6.36</v>
       </c>
       <c r="U334" t="inlineStr">
         <is>
-          <t>28/10/2023 02:28</t>
+          <t>28/10/2023 02:24</t>
         </is>
       </c>
       <c r="V334" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-ponte-preta/EeWldSr9/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-botafogo-sp/QZkfzoMk/</t>
         </is>
       </c>
     </row>
@@ -31209,71 +31209,71 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Guarani</t>
+          <t>Novorizontino</t>
         </is>
       </c>
       <c r="G335" t="n">
+        <v>2</v>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>Ponte Preta</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
         <v>0</v>
       </c>
-      <c r="H335" t="inlineStr">
-        <is>
-          <t>Botafogo SP</t>
-        </is>
-      </c>
-      <c r="I335" t="n">
-        <v>1</v>
-      </c>
       <c r="J335" t="n">
-        <v>1.64</v>
+        <v>1.53</v>
       </c>
       <c r="K335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="L335" t="n">
-        <v>1.7</v>
+        <v>1.39</v>
       </c>
       <c r="M335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:05</t>
+          <t>28/10/2023 02:21</t>
         </is>
       </c>
       <c r="N335" t="n">
-        <v>3.41</v>
+        <v>3.81</v>
       </c>
       <c r="O335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="P335" t="n">
-        <v>3.43</v>
+        <v>4.57</v>
       </c>
       <c r="Q335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:17</t>
+          <t>28/10/2023 02:28</t>
         </is>
       </c>
       <c r="R335" t="n">
-        <v>6.14</v>
+        <v>6.57</v>
       </c>
       <c r="S335" t="inlineStr">
         <is>
-          <t>21/10/2023 22:12</t>
+          <t>24/10/2023 01:12</t>
         </is>
       </c>
       <c r="T335" t="n">
-        <v>6.36</v>
+        <v>10.13</v>
       </c>
       <c r="U335" t="inlineStr">
         <is>
-          <t>28/10/2023 02:24</t>
+          <t>28/10/2023 02:28</t>
         </is>
       </c>
       <c r="V335" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/guarani-botafogo-sp/QZkfzoMk/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/novorizontino-ponte-preta/EeWldSr9/</t>
         </is>
       </c>
     </row>
@@ -33877,71 +33877,71 @@
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Criciuma</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="G364" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H364" t="inlineStr">
         <is>
-          <t>Botafogo SP</t>
+          <t>Sport Recife</t>
         </is>
       </c>
       <c r="I364" t="n">
         <v>0</v>
       </c>
       <c r="J364" t="n">
-        <v>1.48</v>
+        <v>2.36</v>
       </c>
       <c r="K364" t="inlineStr">
         <is>
-          <t>14/11/2023 10:51</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="L364" t="n">
-        <v>1.39</v>
+        <v>2.97</v>
       </c>
       <c r="M364" t="inlineStr">
         <is>
-          <t>18/11/2023 17:56</t>
+          <t>18/11/2023 20:58</t>
         </is>
       </c>
       <c r="N364" t="n">
-        <v>3.79</v>
+        <v>3.3</v>
       </c>
       <c r="O364" t="inlineStr">
         <is>
-          <t>14/11/2023 10:51</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="P364" t="n">
-        <v>4.41</v>
+        <v>3.11</v>
       </c>
       <c r="Q364" t="inlineStr">
         <is>
-          <t>18/11/2023 20:17</t>
+          <t>18/11/2023 20:56</t>
         </is>
       </c>
       <c r="R364" t="n">
-        <v>7.64</v>
+        <v>3.01</v>
       </c>
       <c r="S364" t="inlineStr">
         <is>
-          <t>14/11/2023 10:51</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="T364" t="n">
-        <v>10.7</v>
+        <v>2.67</v>
       </c>
       <c r="U364" t="inlineStr">
         <is>
-          <t>18/11/2023 20:17</t>
+          <t>18/11/2023 20:58</t>
         </is>
       </c>
       <c r="V364" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-botafogo-sp/b9u1suiU/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-sport-recife/WdAF02ih/</t>
         </is>
       </c>
     </row>
@@ -33969,71 +33969,71 @@
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Juventude</t>
+          <t>Vila Nova FC</t>
         </is>
       </c>
       <c r="G365" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Ceara</t>
         </is>
       </c>
       <c r="I365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J365" t="n">
-        <v>1.41</v>
+        <v>1.68</v>
       </c>
       <c r="K365" t="inlineStr">
         <is>
-          <t>14/11/2023 10:52</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="L365" t="n">
-        <v>1.79</v>
+        <v>1.59</v>
       </c>
       <c r="M365" t="inlineStr">
         <is>
-          <t>18/11/2023 20:59</t>
+          <t>18/11/2023 20:56</t>
         </is>
       </c>
       <c r="N365" t="n">
-        <v>4.05</v>
+        <v>3.57</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
-          <t>14/11/2023 10:52</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="P365" t="n">
-        <v>3.29</v>
+        <v>3.79</v>
       </c>
       <c r="Q365" t="inlineStr">
         <is>
-          <t>18/11/2023 20:59</t>
+          <t>18/11/2023 20:56</t>
         </is>
       </c>
       <c r="R365" t="n">
-        <v>8.76</v>
+        <v>5.27</v>
       </c>
       <c r="S365" t="inlineStr">
         <is>
-          <t>14/11/2023 10:52</t>
+          <t>13/11/2023 22:12</t>
         </is>
       </c>
       <c r="T365" t="n">
-        <v>5.76</v>
+        <v>6.96</v>
       </c>
       <c r="U365" t="inlineStr">
         <is>
-          <t>18/11/2023 20:59</t>
+          <t>18/11/2023 20:56</t>
         </is>
       </c>
       <c r="V365" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-ponte-preta/xfDNbtM4/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ceara/KItcrLyO/</t>
         </is>
       </c>
     </row>
@@ -34061,71 +34061,71 @@
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Mirassol</t>
+          <t>Criciuma</t>
         </is>
       </c>
       <c r="G366" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>Atletico GO</t>
+          <t>Botafogo SP</t>
         </is>
       </c>
       <c r="I366" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J366" t="n">
-        <v>1.84</v>
+        <v>1.48</v>
       </c>
       <c r="K366" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:51</t>
         </is>
       </c>
       <c r="L366" t="n">
-        <v>2.28</v>
+        <v>1.39</v>
       </c>
       <c r="M366" t="inlineStr">
         <is>
-          <t>18/11/2023 20:50</t>
+          <t>18/11/2023 17:56</t>
         </is>
       </c>
       <c r="N366" t="n">
-        <v>3.33</v>
+        <v>3.79</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:51</t>
         </is>
       </c>
       <c r="P366" t="n">
-        <v>3.16</v>
+        <v>4.41</v>
       </c>
       <c r="Q366" t="inlineStr">
         <is>
-          <t>18/11/2023 20:56</t>
+          <t>18/11/2023 20:17</t>
         </is>
       </c>
       <c r="R366" t="n">
-        <v>4.96</v>
+        <v>7.64</v>
       </c>
       <c r="S366" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:51</t>
         </is>
       </c>
       <c r="T366" t="n">
-        <v>3.58</v>
+        <v>10.7</v>
       </c>
       <c r="U366" t="inlineStr">
         <is>
-          <t>18/11/2023 20:56</t>
+          <t>18/11/2023 20:17</t>
         </is>
       </c>
       <c r="V366" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-atletico-go/lYKA1rxn/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/criciuma-botafogo-sp/b9u1suiU/</t>
         </is>
       </c>
     </row>
@@ -34153,71 +34153,71 @@
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Vila Nova FC</t>
+          <t>Juventude</t>
         </is>
       </c>
       <c r="G367" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H367" t="inlineStr">
         <is>
-          <t>Ceara</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="I367" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J367" t="n">
-        <v>1.68</v>
+        <v>1.41</v>
       </c>
       <c r="K367" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:52</t>
         </is>
       </c>
       <c r="L367" t="n">
-        <v>1.59</v>
+        <v>1.79</v>
       </c>
       <c r="M367" t="inlineStr">
         <is>
-          <t>18/11/2023 20:56</t>
+          <t>18/11/2023 20:59</t>
         </is>
       </c>
       <c r="N367" t="n">
-        <v>3.57</v>
+        <v>4.05</v>
       </c>
       <c r="O367" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:52</t>
         </is>
       </c>
       <c r="P367" t="n">
-        <v>3.79</v>
+        <v>3.29</v>
       </c>
       <c r="Q367" t="inlineStr">
         <is>
-          <t>18/11/2023 20:56</t>
+          <t>18/11/2023 20:59</t>
         </is>
       </c>
       <c r="R367" t="n">
-        <v>5.27</v>
+        <v>8.76</v>
       </c>
       <c r="S367" t="inlineStr">
         <is>
-          <t>13/11/2023 22:12</t>
+          <t>14/11/2023 10:52</t>
         </is>
       </c>
       <c r="T367" t="n">
-        <v>6.96</v>
+        <v>5.76</v>
       </c>
       <c r="U367" t="inlineStr">
         <is>
-          <t>18/11/2023 20:56</t>
+          <t>18/11/2023 20:59</t>
         </is>
       </c>
       <c r="V367" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vila-nova-fc-ceara/KItcrLyO/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/esporte-clube-juventude-ponte-preta/xfDNbtM4/</t>
         </is>
       </c>
     </row>
@@ -34245,22 +34245,22 @@
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Mirassol</t>
         </is>
       </c>
       <c r="G368" t="n">
+        <v>4</v>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>Atletico GO</t>
+        </is>
+      </c>
+      <c r="I368" t="n">
         <v>1</v>
       </c>
-      <c r="H368" t="inlineStr">
-        <is>
-          <t>Sport Recife</t>
-        </is>
-      </c>
-      <c r="I368" t="n">
-        <v>0</v>
-      </c>
       <c r="J368" t="n">
-        <v>2.36</v>
+        <v>1.84</v>
       </c>
       <c r="K368" t="inlineStr">
         <is>
@@ -34268,15 +34268,15 @@
         </is>
       </c>
       <c r="L368" t="n">
-        <v>2.97</v>
+        <v>2.28</v>
       </c>
       <c r="M368" t="inlineStr">
         <is>
-          <t>18/11/2023 20:58</t>
+          <t>18/11/2023 20:50</t>
         </is>
       </c>
       <c r="N368" t="n">
-        <v>3.3</v>
+        <v>3.33</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
@@ -34284,7 +34284,7 @@
         </is>
       </c>
       <c r="P368" t="n">
-        <v>3.11</v>
+        <v>3.16</v>
       </c>
       <c r="Q368" t="inlineStr">
         <is>
@@ -34292,7 +34292,7 @@
         </is>
       </c>
       <c r="R368" t="n">
-        <v>3.01</v>
+        <v>4.96</v>
       </c>
       <c r="S368" t="inlineStr">
         <is>
@@ -34300,16 +34300,16 @@
         </is>
       </c>
       <c r="T368" t="n">
-        <v>2.67</v>
+        <v>3.58</v>
       </c>
       <c r="U368" t="inlineStr">
         <is>
-          <t>18/11/2023 20:58</t>
+          <t>18/11/2023 20:56</t>
         </is>
       </c>
       <c r="V368" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-b/vitoria-sport-recife/WdAF02ih/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/mirassol-atletico-go/lYKA1rxn/</t>
         </is>
       </c>
     </row>
@@ -34494,6 +34494,98 @@
       <c r="V370" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/brazil/serie-b/crb-tombense/YL6WdKjH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>serie-b</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E371" s="2" t="n">
+        <v>45251</v>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>Sampaio Correa</t>
+        </is>
+      </c>
+      <c r="G371" t="n">
+        <v>4</v>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>Avai</t>
+        </is>
+      </c>
+      <c r="I371" t="n">
+        <v>0</v>
+      </c>
+      <c r="J371" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="K371" t="inlineStr">
+        <is>
+          <t>14/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L371" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="M371" t="inlineStr">
+        <is>
+          <t>20/11/2023 23:55</t>
+        </is>
+      </c>
+      <c r="N371" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="O371" t="inlineStr">
+        <is>
+          <t>14/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P371" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Q371" t="inlineStr">
+        <is>
+          <t>20/11/2023 23:56</t>
+        </is>
+      </c>
+      <c r="R371" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="S371" t="inlineStr">
+        <is>
+          <t>14/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T371" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="U371" t="inlineStr">
+        <is>
+          <t>20/11/2023 23:43</t>
+        </is>
+      </c>
+      <c r="V371" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-b/sampaio-correa-avai/rXDJaM6b/</t>
         </is>
       </c>
     </row>

</xml_diff>